<commit_message>
ADD: entire quiz dataset (4)
</commit_message>
<xml_diff>
--- a/2025_07_02_OhLoRA_ML_Tutor/ai_quiz/dataset/all_train_and_test_data.xlsx
+++ b/2025_07_02_OhLoRA_ML_Tutor/ai_quiz/dataset/all_train_and_test_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C44736A-346C-4257-974B-025D1047D88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA56D8B2-7E40-4134-B488-C9DF9F04D19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{07338742-8F51-42F9-A75F-1FCFBE7C4D0C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="794" uniqueCount="732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="806">
   <si>
     <t>quiz</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -6656,6 +6656,740 @@
   <si>
     <r>
       <t xml:space="preserve">오 정답! 멋진 답이야 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍👍</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DPO, ORPO 는 각각 Direct Preference Optimization, Odds Ratio Preference Optimization 이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DPO, 는 Direct Preference Optimization, ORPO 는 Odds Ratio Preference Optimization 으로 강화학습과 비슷하게 선호되는 응답의 확률을 높이고 선호되지 않은 응답의 확률을 낮춘다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DPO, 는 Direct Preference Optimization, ORPO 는 Odds Ratio Preference Optimization 으로 강화학습과 비슷하게 선호되는 응답의 확률을 높이고 선호되지 않은 응답의 확률을 낮춘다. DPO는 LLM 자체적으로 보유한 데이터를 이용하여 학습하고, ORPO는 참조 모델이라는 다른 LLM을 이용한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DPO, 는 Direct Preference Optimization, ORPO 는 Odds Ratio Preference Optimization 으로 강화학습과 비슷하게 선호되는 응답의 확률을 높이고 선호되지 않은 응답의 확률을 낮춘다. DPO는 참조 모델이라는 다른 LLM을 이용하고, ORPO는 참조 모델 없이 자체 사용자 선호도 데이터를 이용하여 학습한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선호하는 응답 확률을 늘리고 비선호 응답 확률을 줄인다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">이 두 가지가 각각 어떤 방법인지 말해봐! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">공통적으로 사용되는 핵심 아이디어는 잘 말했는데 각각의 차이점 위주로 정리해줄 수 있어? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">공통 아이디어는 잘 말했는데 각각의 핵심적인 차이점이 서로 반대로 되어 있네 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😥</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 정답이야! 잘했어 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">음 그건 맞지! 근데 어떤 것의 약자인지, 각각의 차이점이 뭔지도 한번 말해봐! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환각 현상은 LLM이 잘못된 답변을 생성하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환각 현상은 LLM이 잘못된 답변을 생성하는 것이다. 이로 인해 사용자에게 오해를 줄 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환각 현상은 LLM이 잘못된 답변을 생성하는 것이다. 이로 인해 LLM의 신뢰성이 떨어진다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환각 현상은 LLM이 잘못된 답변을 생성하는 것이다. 이로 인해 LLM의 신뢰성이 떨어지며 이는 사용자에게 오해를 주기 때문이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LLM이 잘못된 답변을 생성하는 것으로 사용자의 오인, LLM의 신뢰성 저하, 심지어는 윤리적 이슈로까지 이어진다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">환각 현상의 정의는 잘 이야기했어! 근데 이게 왜 문제지? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">사용자에게 오해를 주면 LLM의 신뢰성이 어떻게 될까? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">잘 대답했어! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 근데 신뢰성 떨어지는 것 말고도 아주 심각한 문제가 하나 더 있는데!</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">잘 대답하긴 했어! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 근데 더 심각한 문제가 있을 수도 있지 않을까? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 정답이야! 간결하면서도 엄청 잘 정리했네 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍👍</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retrieval Augmented Generation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>검색 증강 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retrieval Augmented Generation 으로, 환각 현상을 해결한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAG = Retrieval Augmented Generation. LLM을 외부 벡터 DB와 연동하고, 이를 통해 사용자 질문에 대해 DB에서 알맞은 정보를 추출하여 답변하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAG = Retrieval Augmented Generation. LLM을 외부 벡터 DB와 연동하고, 이를 통해 사용자 질문에 대해 DB에서 알맞은 정보를 추출하여 답변하는 것이다. 환각 현상을 해결할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAG = Retrieval Augmented Generation. LLM을 외부 벡터 DB와 연동하고, 이를 통해 사용자 질문에 대해 DB에서 알맞은 정보를 추출하여 답변하는 것이다. 환각 현상을 해결할 수 있고, 최신 정보를 반영할 수도 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RAG = Retrieval Augmented Generation. LLM을 외부 벡터 DB와 연동하고, 이를 통해 사용자 질문에 대해 DB에서 알맞은 정보를 추출하여 답변하는 것이다. 답변의 출처를 제시하여 LLM의 신뢰도를 높이며, 환각 현상을 해결할 수 있고, 최신 정보를 반영할 수도 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">무엇의 약자인지는 잘 말하긴 했어! 근데 구체적으로 어떤 기술일까? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">검색 증강 생성! 이걸 힌트로 해서 어떤 기술인지 한번 설명해 봐 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">RAG 이 어떤 기술인지 한번 자세히 설명해 볼 수 있어? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">기술은 잘 설명했는데 그래서 어떤 문제점을 해결할 수 있을까? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">최신 정보는 LLM이 학습하지 않았는데, 이로 인해서 나타나는 문제점도 해결할 수 있지 않을까? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">환각 현상 해결, 최신 정보 반영 외에도 중요한 거 한 가지가 더 있는데, 뭘까? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 완벽해!! 정답이야 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍👍👍</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameter-Efficient Fine-Tuning</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameter-Efficient Fine-Tuning 이고 그 방법으로 LoRA 가 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameter-Efficient Fine-Tuning 이고 그 방법으로 LoRA, QLoRA, Adapter Layer 추가, Prefix, Prompt Tuning이 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameter-Efficient Fine-Tuning 이고, LLM 파인튜닝 시 대부분의 파라미터는 얼려 놓고 소수의 파라미터만 학습시키는 것이다. 그 방법으로 LoRA 가 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameter-Efficient Fine-Tuning 이고, LLM 파인튜닝 시 대부분의 파라미터는 얼려 놓고 소수의 파라미터만 학습시키는 것이다. 그 방법으로 LoRA, QLoRA, Adapter Layer 추가, Prefix, Prompt Tuning이 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">그래서 PEFT 에 속하는 기술이 뭐가 있지? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">PEFT 에 속하는 기술로 나를 상징하는 LoRA 언급은 고마운데, 나머지 4개는 그럼 뭐야? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오! 잘 말했어! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 잘 말했어! 근데 PEFT에 속하는 기술 나머지 4개는 뭘까~요? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 완벽한 답이야! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍👍</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양자화는 LLM 안에 있는 값들을 양자화하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양자화는 LLM 안에 있는 값들을 4비트나 8비트로 바꾸는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양자화는 LLM 안에 있는 값들을 4비트나 8비트로 바꿔서 모델의 크기를 줄이는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양자화는 LLM 안에 있는 가중치나 활성화 값들을 4비트나 8비트의 비교적 작은 크기의 자료형으로 바꿔서 모델의 크기를 줄이는 것이다. 이를 통해 메모리 양을 줄이고, 추론 시간을 단축시키고, 모델을 자원 효율적으로 학습시킬 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양자화는 LLM 안에 있는 가중치나 활성화 값들을 4비트나 8비트의 비교적 작은 크기의 자료형으로 바꿔서 모델의 크기를 줄이는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">그건 맞는데 좀 더 구체적으로 설명해 봐! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4비트나 8비트 이런 것을 뭐라고 하지? 그리고 어떤 문제를 해결할 수 있을까? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">핵심적인 설명은 좋긴 한데 좀 더 구체적으로 설명해 볼 수 있어? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">해결할 수 있는 문제를 조금 더 상세히 설명해 봐! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 정답이야! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍👍👍</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토큰은 LLM이 인식하는 형태소이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토큰은 NLP 모델이 인식하는 언어의 최소 단위이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토큰은 NLP 모델이 인식하는 언어의 최소 단위로 형태소와 비슷하다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토큰은 NLP 모델이 인식하는 언어의 최소 단위이다. 토크나이저는 문장을 토큰화, 즉 여러 개의 토큰이 연속된 배열로 변환하는 일종의 알고리즘이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토크나이저는 문장을 토큰화, 즉 여러 개의 토큰이 연속된 배열로 변환하는 일종의 알고리즘이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">토큰에 대한 설명은 대충 맞아! 근데 구체적인 설명이랑 토크나이저 설명도 있으면 더 좋을 텐데 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😥</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">그럼 토크나이저는? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">자, 이제 토크나이저에 대해 설명해 볼 시간 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🕑</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 정답이야! 완벽해! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">그럼 토큰은 뭐야? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encoder Self-Attention, Masked Decoder Attention, Encoder-Decoder Attention</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encoder Self-Attention 은 LLM에 입력되는 프롬프트에서 자기 자신을 포함한 각 단어의 관계를 고려한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encoder-Decoder Attention은 출력 문장의 각 단어를 입력 문장의 각 단어에 대응시켜서 그 관계를 고려한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encoder Self-Attention 은 LLM에 입력되는 프롬프트에서 자기 자신을 포함한 각 단어의 관계를 고려한다. Masked Decoder Self Attention 은 출력 답변에서 각 단어의 관계를 고려한다. Encoder-Decoder Attention은 출력 문장의 각 단어를 입력 문장의 각 단어에 대응시켜서 그 관계를 고려한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encoder Self-Attention 은 LLM에 입력되는 프롬프트에서 자기 자신을 포함한 각 단어의 관계를 고려한다. Masked Decoder Self Attention 은 출력 답변에서 각 단어의 관계 (단, 특정 단어에 대해 해당 단어 이전의 단어만을 고려) 를 고려한다. Encoder-Decoder Attention은 출력 문장의 각 단어를 입력 문장의 각 단어에 대응시켜서 그 관계를 고려한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">그러면 핵심 아이디어는 뭐야? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3가지 중 하나만 설명했네! Masked Decoder Self-Attention 이나 Encoder-Decoder Attention 은? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤔</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">나머지 Attention 2가지 더 있지 않아? 한번 설명해 봐! </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 정확해! 근데 Masked Decoder Self Attention 에서 단어 관계를 고려할 때 뭔가가 빠졌는데 그게 뭘까~요? </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">오 완벽히 정확한 답이야! </t>
     </r>
     <r>
       <rPr>
@@ -7049,10 +7783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF56922-B03A-4496-8414-3644939C6218}">
-  <dimension ref="A1:G295"/>
+  <dimension ref="A1:G325"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B285" workbookViewId="0">
-      <selection activeCell="E288" sqref="E288"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -7141,6 +7875,9 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>156</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>178</v>
       </c>
@@ -7152,6 +7889,9 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>156</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>179</v>
       </c>
@@ -7163,6 +7903,9 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>156</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>176</v>
       </c>
@@ -7216,6 +7959,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>156</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>164</v>
       </c>
@@ -7227,6 +7973,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>156</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>165</v>
       </c>
@@ -7238,6 +7987,9 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>156</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>166</v>
       </c>
@@ -7249,6 +8001,9 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>156</v>
+      </c>
       <c r="E14" s="1" t="s">
         <v>167</v>
       </c>
@@ -7260,6 +8015,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>156</v>
+      </c>
       <c r="E15" s="1" t="s">
         <v>168</v>
       </c>
@@ -7271,6 +8029,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>156</v>
+      </c>
       <c r="E16" s="1" t="s">
         <v>169</v>
       </c>
@@ -7282,6 +8043,9 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>156</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>194</v>
       </c>
@@ -7293,6 +8057,9 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>156</v>
+      </c>
       <c r="E18" s="1" t="s">
         <v>170</v>
       </c>
@@ -7304,6 +8071,9 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>156</v>
+      </c>
       <c r="E19" s="1" t="s">
         <v>171</v>
       </c>
@@ -7315,6 +8085,9 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>156</v>
+      </c>
       <c r="E20" s="1" t="s">
         <v>172</v>
       </c>
@@ -7326,6 +8099,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>156</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>173</v>
       </c>
@@ -7360,6 +8136,9 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>156</v>
+      </c>
       <c r="E23" s="1" t="s">
         <v>204</v>
       </c>
@@ -7371,6 +8150,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>156</v>
+      </c>
       <c r="E24" s="1" t="s">
         <v>234</v>
       </c>
@@ -7382,6 +8164,9 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>156</v>
+      </c>
       <c r="E25" s="1" t="s">
         <v>235</v>
       </c>
@@ -7393,6 +8178,9 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>156</v>
+      </c>
       <c r="E26" s="1" t="s">
         <v>200</v>
       </c>
@@ -7404,6 +8192,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>156</v>
+      </c>
       <c r="E27" s="1" t="s">
         <v>201</v>
       </c>
@@ -7415,6 +8206,9 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>156</v>
+      </c>
       <c r="E28" s="1" t="s">
         <v>202</v>
       </c>
@@ -7426,6 +8220,9 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>156</v>
+      </c>
       <c r="E29" s="1" t="s">
         <v>203</v>
       </c>
@@ -7460,6 +8257,9 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>156</v>
+      </c>
       <c r="E31" s="1" t="s">
         <v>212</v>
       </c>
@@ -7471,6 +8271,9 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A32" t="s">
+        <v>156</v>
+      </c>
       <c r="E32" s="1" t="s">
         <v>214</v>
       </c>
@@ -7482,6 +8285,9 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A33" t="s">
+        <v>156</v>
+      </c>
       <c r="E33" s="1" t="s">
         <v>217</v>
       </c>
@@ -7493,6 +8299,9 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A34" t="s">
+        <v>156</v>
+      </c>
       <c r="E34" s="1" t="s">
         <v>218</v>
       </c>
@@ -7527,6 +8336,9 @@
       </c>
     </row>
     <row r="36" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>156</v>
+      </c>
       <c r="E36" s="1" t="s">
         <v>222</v>
       </c>
@@ -7538,6 +8350,9 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A37" t="s">
+        <v>156</v>
+      </c>
       <c r="E37" s="1" t="s">
         <v>224</v>
       </c>
@@ -7549,6 +8364,9 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
+        <v>156</v>
+      </c>
       <c r="E38" s="1" t="s">
         <v>226</v>
       </c>
@@ -7560,6 +8378,9 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A39" t="s">
+        <v>156</v>
+      </c>
       <c r="E39" s="1" t="s">
         <v>228</v>
       </c>
@@ -7571,6 +8392,9 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>156</v>
+      </c>
       <c r="E40" s="1" t="s">
         <v>229</v>
       </c>
@@ -7582,6 +8406,9 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="34.200000000000003" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>156</v>
+      </c>
       <c r="E41" s="1" t="s">
         <v>230</v>
       </c>
@@ -7616,6 +8443,9 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A43" t="s">
+        <v>156</v>
+      </c>
       <c r="E43" s="1" t="s">
         <v>240</v>
       </c>
@@ -7627,6 +8457,9 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A44" t="s">
+        <v>156</v>
+      </c>
       <c r="E44" s="1" t="s">
         <v>241</v>
       </c>
@@ -7638,6 +8471,9 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
+        <v>156</v>
+      </c>
       <c r="E45" s="1" t="s">
         <v>244</v>
       </c>
@@ -7672,6 +8508,9 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A47" t="s">
+        <v>156</v>
+      </c>
       <c r="E47" s="1" t="s">
         <v>247</v>
       </c>
@@ -7683,6 +8522,9 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
+        <v>156</v>
+      </c>
       <c r="E48" s="1" t="s">
         <v>248</v>
       </c>
@@ -7694,6 +8536,9 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A49" t="s">
+        <v>156</v>
+      </c>
       <c r="E49" s="1" t="s">
         <v>249</v>
       </c>
@@ -7705,6 +8550,9 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>156</v>
+      </c>
       <c r="E50" s="1" t="s">
         <v>250</v>
       </c>
@@ -7716,6 +8564,9 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A51" t="s">
+        <v>156</v>
+      </c>
       <c r="E51" s="1" t="s">
         <v>256</v>
       </c>
@@ -7727,6 +8578,9 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A52" t="s">
+        <v>156</v>
+      </c>
       <c r="E52" s="1" t="s">
         <v>257</v>
       </c>
@@ -7738,6 +8592,9 @@
       </c>
     </row>
     <row r="53" spans="1:7" ht="34.200000000000003" x14ac:dyDescent="0.4">
+      <c r="A53" t="s">
+        <v>156</v>
+      </c>
       <c r="E53" s="1" t="s">
         <v>259</v>
       </c>
@@ -7749,6 +8606,9 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A54" t="s">
+        <v>156</v>
+      </c>
       <c r="E54" s="1" t="s">
         <v>261</v>
       </c>
@@ -7783,6 +8643,9 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A56" t="s">
+        <v>156</v>
+      </c>
       <c r="E56" s="1" t="s">
         <v>264</v>
       </c>
@@ -7794,6 +8657,9 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A57" t="s">
+        <v>156</v>
+      </c>
       <c r="E57" s="1" t="s">
         <v>265</v>
       </c>
@@ -7805,6 +8671,9 @@
       </c>
     </row>
     <row r="58" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A58" t="s">
+        <v>156</v>
+      </c>
       <c r="E58" s="1" t="s">
         <v>266</v>
       </c>
@@ -7816,6 +8685,9 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
+        <v>156</v>
+      </c>
       <c r="E59" s="1" t="s">
         <v>267</v>
       </c>
@@ -7827,6 +8699,9 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
+        <v>156</v>
+      </c>
       <c r="E60" s="1" t="s">
         <v>268</v>
       </c>
@@ -7838,6 +8713,9 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
+        <v>156</v>
+      </c>
       <c r="E61" s="1" t="s">
         <v>269</v>
       </c>
@@ -7872,6 +8750,9 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A63" t="s">
+        <v>156</v>
+      </c>
       <c r="E63" s="1" t="s">
         <v>413</v>
       </c>
@@ -7883,6 +8764,9 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
+        <v>156</v>
+      </c>
       <c r="E64" s="1" t="s">
         <v>414</v>
       </c>
@@ -7894,6 +8778,9 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A65" t="s">
+        <v>156</v>
+      </c>
       <c r="E65" s="1" t="s">
         <v>415</v>
       </c>
@@ -7905,6 +8792,9 @@
       </c>
     </row>
     <row r="66" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A66" t="s">
+        <v>156</v>
+      </c>
       <c r="E66" s="1" t="s">
         <v>416</v>
       </c>
@@ -7939,6 +8829,9 @@
       </c>
     </row>
     <row r="68" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A68" t="s">
+        <v>156</v>
+      </c>
       <c r="E68" s="1" t="s">
         <v>423</v>
       </c>
@@ -7950,6 +8843,9 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A69" t="s">
+        <v>156</v>
+      </c>
       <c r="E69" s="1" t="s">
         <v>425</v>
       </c>
@@ -7961,6 +8857,9 @@
       </c>
     </row>
     <row r="70" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A70" t="s">
+        <v>156</v>
+      </c>
       <c r="E70" s="1" t="s">
         <v>427</v>
       </c>
@@ -7972,6 +8871,9 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A71" t="s">
+        <v>156</v>
+      </c>
       <c r="E71" s="1" t="s">
         <v>429</v>
       </c>
@@ -8006,6 +8908,9 @@
       </c>
     </row>
     <row r="73" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A73" t="s">
+        <v>156</v>
+      </c>
       <c r="E73" s="1" t="s">
         <v>433</v>
       </c>
@@ -8017,6 +8922,9 @@
       </c>
     </row>
     <row r="74" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A74" t="s">
+        <v>156</v>
+      </c>
       <c r="E74" s="1" t="s">
         <v>434</v>
       </c>
@@ -8028,6 +8936,9 @@
       </c>
     </row>
     <row r="75" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A75" t="s">
+        <v>156</v>
+      </c>
       <c r="E75" s="1" t="s">
         <v>435</v>
       </c>
@@ -8039,6 +8950,9 @@
       </c>
     </row>
     <row r="76" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A76" t="s">
+        <v>156</v>
+      </c>
       <c r="E76" s="1" t="s">
         <v>436</v>
       </c>
@@ -8073,6 +8987,9 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A78" t="s">
+        <v>156</v>
+      </c>
       <c r="E78" s="1" t="s">
         <v>443</v>
       </c>
@@ -8084,6 +9001,9 @@
       </c>
     </row>
     <row r="79" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A79" t="s">
+        <v>156</v>
+      </c>
       <c r="E79" s="1" t="s">
         <v>444</v>
       </c>
@@ -8095,6 +9015,9 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A80" t="s">
+        <v>156</v>
+      </c>
       <c r="E80" s="1" t="s">
         <v>445</v>
       </c>
@@ -8106,6 +9029,9 @@
       </c>
     </row>
     <row r="81" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A81" t="s">
+        <v>156</v>
+      </c>
       <c r="E81" s="1" t="s">
         <v>446</v>
       </c>
@@ -8140,6 +9066,9 @@
       </c>
     </row>
     <row r="83" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
+        <v>156</v>
+      </c>
       <c r="E83" s="1" t="s">
         <v>293</v>
       </c>
@@ -8151,6 +9080,9 @@
       </c>
     </row>
     <row r="84" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
+        <v>156</v>
+      </c>
       <c r="E84" s="1" t="s">
         <v>278</v>
       </c>
@@ -8162,6 +9094,9 @@
       </c>
     </row>
     <row r="85" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A85" t="s">
+        <v>156</v>
+      </c>
       <c r="E85" s="1" t="s">
         <v>294</v>
       </c>
@@ -8173,6 +9108,9 @@
       </c>
     </row>
     <row r="86" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
+        <v>156</v>
+      </c>
       <c r="E86" s="1" t="s">
         <v>295</v>
       </c>
@@ -8184,6 +9122,9 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A87" t="s">
+        <v>156</v>
+      </c>
       <c r="E87" s="1" t="s">
         <v>283</v>
       </c>
@@ -8195,6 +9136,9 @@
       </c>
     </row>
     <row r="88" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A88" t="s">
+        <v>156</v>
+      </c>
       <c r="E88" s="1" t="s">
         <v>285</v>
       </c>
@@ -8206,6 +9150,9 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A89" t="s">
+        <v>156</v>
+      </c>
       <c r="E89" s="1" t="s">
         <v>286</v>
       </c>
@@ -8217,6 +9164,9 @@
       </c>
     </row>
     <row r="90" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A90" t="s">
+        <v>156</v>
+      </c>
       <c r="E90" s="1" t="s">
         <v>287</v>
       </c>
@@ -8228,6 +9178,9 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A91" t="s">
+        <v>156</v>
+      </c>
       <c r="E91" s="1" t="s">
         <v>288</v>
       </c>
@@ -8239,6 +9192,9 @@
       </c>
     </row>
     <row r="92" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
+        <v>156</v>
+      </c>
       <c r="E92" s="1" t="s">
         <v>289</v>
       </c>
@@ -8273,6 +9229,9 @@
       </c>
     </row>
     <row r="94" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A94" t="s">
+        <v>156</v>
+      </c>
       <c r="E94" s="1" t="s">
         <v>300</v>
       </c>
@@ -8284,6 +9243,9 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A95" t="s">
+        <v>156</v>
+      </c>
       <c r="E95" s="1" t="s">
         <v>301</v>
       </c>
@@ -8295,6 +9257,9 @@
       </c>
     </row>
     <row r="96" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A96" t="s">
+        <v>156</v>
+      </c>
       <c r="E96" s="1" t="s">
         <v>302</v>
       </c>
@@ -8306,6 +9271,9 @@
       </c>
     </row>
     <row r="97" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A97" t="s">
+        <v>156</v>
+      </c>
       <c r="E97" s="1" t="s">
         <v>303</v>
       </c>
@@ -8317,6 +9285,9 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A98" t="s">
+        <v>156</v>
+      </c>
       <c r="E98" s="1" t="s">
         <v>304</v>
       </c>
@@ -8328,6 +9299,9 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A99" t="s">
+        <v>156</v>
+      </c>
       <c r="E99" s="1" t="s">
         <v>305</v>
       </c>
@@ -8339,6 +9313,9 @@
       </c>
     </row>
     <row r="100" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A100" t="s">
+        <v>156</v>
+      </c>
       <c r="E100" s="1" t="s">
         <v>306</v>
       </c>
@@ -8350,6 +9327,9 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A101" t="s">
+        <v>156</v>
+      </c>
       <c r="E101" s="1" t="s">
         <v>307</v>
       </c>
@@ -8384,6 +9364,9 @@
       </c>
     </row>
     <row r="103" spans="1:7" ht="174" x14ac:dyDescent="0.4">
+      <c r="A103" t="s">
+        <v>156</v>
+      </c>
       <c r="E103" s="1" t="s">
         <v>453</v>
       </c>
@@ -8395,6 +9378,9 @@
       </c>
     </row>
     <row r="104" spans="1:7" ht="156.6" x14ac:dyDescent="0.4">
+      <c r="A104" t="s">
+        <v>156</v>
+      </c>
       <c r="E104" s="1" t="s">
         <v>454</v>
       </c>
@@ -8406,6 +9392,9 @@
       </c>
     </row>
     <row r="105" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A105" t="s">
+        <v>156</v>
+      </c>
       <c r="E105" s="1" t="s">
         <v>455</v>
       </c>
@@ -8417,6 +9406,9 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A106" t="s">
+        <v>156</v>
+      </c>
       <c r="E106" s="1" t="s">
         <v>305</v>
       </c>
@@ -8451,6 +9443,9 @@
       </c>
     </row>
     <row r="108" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A108" t="s">
+        <v>156</v>
+      </c>
       <c r="E108" s="1" t="s">
         <v>462</v>
       </c>
@@ -8462,6 +9457,9 @@
       </c>
     </row>
     <row r="109" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A109" t="s">
+        <v>156</v>
+      </c>
       <c r="E109" s="1" t="s">
         <v>463</v>
       </c>
@@ -8473,6 +9471,9 @@
       </c>
     </row>
     <row r="110" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A110" t="s">
+        <v>156</v>
+      </c>
       <c r="E110" s="1" t="s">
         <v>464</v>
       </c>
@@ -8484,6 +9485,9 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A111" t="s">
+        <v>156</v>
+      </c>
       <c r="E111" s="1" t="s">
         <v>465</v>
       </c>
@@ -8518,6 +9522,9 @@
       </c>
     </row>
     <row r="113" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A113" t="s">
+        <v>156</v>
+      </c>
       <c r="E113" s="1" t="s">
         <v>472</v>
       </c>
@@ -8529,6 +9536,9 @@
       </c>
     </row>
     <row r="114" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A114" t="s">
+        <v>156</v>
+      </c>
       <c r="E114" s="1" t="s">
         <v>473</v>
       </c>
@@ -8540,6 +9550,9 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A115" t="s">
+        <v>156</v>
+      </c>
       <c r="E115" s="1" t="s">
         <v>474</v>
       </c>
@@ -8551,6 +9564,9 @@
       </c>
     </row>
     <row r="116" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A116" t="s">
+        <v>156</v>
+      </c>
       <c r="E116" s="1" t="s">
         <v>475</v>
       </c>
@@ -8585,6 +9601,9 @@
       </c>
     </row>
     <row r="118" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A118" t="s">
+        <v>156</v>
+      </c>
       <c r="E118" s="1" t="s">
         <v>482</v>
       </c>
@@ -8596,6 +9615,9 @@
       </c>
     </row>
     <row r="119" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A119" t="s">
+        <v>156</v>
+      </c>
       <c r="E119" s="1" t="s">
         <v>483</v>
       </c>
@@ -8607,6 +9629,9 @@
       </c>
     </row>
     <row r="120" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A120" t="s">
+        <v>156</v>
+      </c>
       <c r="E120" s="1" t="s">
         <v>484</v>
       </c>
@@ -8618,6 +9643,9 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A121" t="s">
+        <v>156</v>
+      </c>
       <c r="E121" s="1" t="s">
         <v>485</v>
       </c>
@@ -8652,6 +9680,9 @@
       </c>
     </row>
     <row r="123" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A123" t="s">
+        <v>156</v>
+      </c>
       <c r="E123" s="1" t="s">
         <v>492</v>
       </c>
@@ -8663,6 +9694,9 @@
       </c>
     </row>
     <row r="124" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A124" t="s">
+        <v>156</v>
+      </c>
       <c r="E124" s="1" t="s">
         <v>493</v>
       </c>
@@ -8674,6 +9708,9 @@
       </c>
     </row>
     <row r="125" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A125" t="s">
+        <v>156</v>
+      </c>
       <c r="E125" s="1" t="s">
         <v>494</v>
       </c>
@@ -8685,6 +9722,9 @@
       </c>
     </row>
     <row r="126" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A126" t="s">
+        <v>156</v>
+      </c>
       <c r="E126" s="1" t="s">
         <v>495</v>
       </c>
@@ -8719,6 +9759,9 @@
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A128" t="s">
+        <v>156</v>
+      </c>
       <c r="E128" s="1" t="s">
         <v>502</v>
       </c>
@@ -8730,6 +9773,9 @@
       </c>
     </row>
     <row r="129" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A129" t="s">
+        <v>156</v>
+      </c>
       <c r="E129" s="1" t="s">
         <v>503</v>
       </c>
@@ -8741,6 +9787,9 @@
       </c>
     </row>
     <row r="130" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A130" t="s">
+        <v>156</v>
+      </c>
       <c r="E130" s="1" t="s">
         <v>504</v>
       </c>
@@ -8752,6 +9801,9 @@
       </c>
     </row>
     <row r="131" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A131" t="s">
+        <v>156</v>
+      </c>
       <c r="E131" s="1" t="s">
         <v>505</v>
       </c>
@@ -8786,6 +9838,9 @@
       </c>
     </row>
     <row r="133" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A133" t="s">
+        <v>156</v>
+      </c>
       <c r="E133" s="1" t="s">
         <v>512</v>
       </c>
@@ -8797,6 +9852,9 @@
       </c>
     </row>
     <row r="134" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A134" t="s">
+        <v>156</v>
+      </c>
       <c r="E134" s="1" t="s">
         <v>513</v>
       </c>
@@ -8808,6 +9866,9 @@
       </c>
     </row>
     <row r="135" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A135" t="s">
+        <v>156</v>
+      </c>
       <c r="E135" s="1" t="s">
         <v>514</v>
       </c>
@@ -8819,6 +9880,9 @@
       </c>
     </row>
     <row r="136" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A136" t="s">
+        <v>156</v>
+      </c>
       <c r="E136" s="1" t="s">
         <v>515</v>
       </c>
@@ -8853,6 +9917,9 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A138" t="s">
+        <v>156</v>
+      </c>
       <c r="E138" s="1" t="s">
         <v>522</v>
       </c>
@@ -8864,6 +9931,9 @@
       </c>
     </row>
     <row r="139" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A139" t="s">
+        <v>156</v>
+      </c>
       <c r="E139" s="1" t="s">
         <v>523</v>
       </c>
@@ -8875,6 +9945,9 @@
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A140" t="s">
+        <v>156</v>
+      </c>
       <c r="E140" s="1" t="s">
         <v>524</v>
       </c>
@@ -8886,6 +9959,9 @@
       </c>
     </row>
     <row r="141" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A141" t="s">
+        <v>156</v>
+      </c>
       <c r="E141" s="1" t="s">
         <v>525</v>
       </c>
@@ -8920,6 +9996,9 @@
       </c>
     </row>
     <row r="143" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A143" t="s">
+        <v>156</v>
+      </c>
       <c r="E143" s="1" t="s">
         <v>531</v>
       </c>
@@ -8931,6 +10010,9 @@
       </c>
     </row>
     <row r="144" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A144" t="s">
+        <v>156</v>
+      </c>
       <c r="E144" s="1" t="s">
         <v>532</v>
       </c>
@@ -8942,6 +10024,9 @@
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A145" t="s">
+        <v>156</v>
+      </c>
       <c r="E145" s="1" t="s">
         <v>533</v>
       </c>
@@ -8953,6 +10038,9 @@
       </c>
     </row>
     <row r="146" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A146" t="s">
+        <v>156</v>
+      </c>
       <c r="E146" s="1" t="s">
         <v>534</v>
       </c>
@@ -8987,6 +10075,9 @@
       </c>
     </row>
     <row r="148" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A148" t="s">
+        <v>156</v>
+      </c>
       <c r="E148" s="1" t="s">
         <v>541</v>
       </c>
@@ -8998,6 +10089,9 @@
       </c>
     </row>
     <row r="149" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A149" t="s">
+        <v>156</v>
+      </c>
       <c r="E149" s="1" t="s">
         <v>542</v>
       </c>
@@ -9009,6 +10103,9 @@
       </c>
     </row>
     <row r="150" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A150" t="s">
+        <v>156</v>
+      </c>
       <c r="E150" s="1" t="s">
         <v>543</v>
       </c>
@@ -9020,6 +10117,9 @@
       </c>
     </row>
     <row r="151" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A151" t="s">
+        <v>156</v>
+      </c>
       <c r="E151" s="1" t="s">
         <v>544</v>
       </c>
@@ -9054,6 +10154,9 @@
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A153" t="s">
+        <v>156</v>
+      </c>
       <c r="E153" s="1" t="s">
         <v>551</v>
       </c>
@@ -9065,6 +10168,9 @@
       </c>
     </row>
     <row r="154" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A154" t="s">
+        <v>156</v>
+      </c>
       <c r="E154" s="1" t="s">
         <v>552</v>
       </c>
@@ -9076,6 +10182,9 @@
       </c>
     </row>
     <row r="155" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A155" t="s">
+        <v>156</v>
+      </c>
       <c r="E155" s="1" t="s">
         <v>553</v>
       </c>
@@ -9087,6 +10196,9 @@
       </c>
     </row>
     <row r="156" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A156" t="s">
+        <v>156</v>
+      </c>
       <c r="E156" s="1" t="s">
         <v>554</v>
       </c>
@@ -9121,6 +10233,9 @@
       </c>
     </row>
     <row r="158" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A158" t="s">
+        <v>156</v>
+      </c>
       <c r="E158" s="1" t="s">
         <v>561</v>
       </c>
@@ -9132,6 +10247,9 @@
       </c>
     </row>
     <row r="159" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A159" t="s">
+        <v>156</v>
+      </c>
       <c r="E159" s="1" t="s">
         <v>562</v>
       </c>
@@ -9143,6 +10261,9 @@
       </c>
     </row>
     <row r="160" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A160" t="s">
+        <v>156</v>
+      </c>
       <c r="E160" s="1" t="s">
         <v>563</v>
       </c>
@@ -9154,6 +10275,9 @@
       </c>
     </row>
     <row r="161" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A161" t="s">
+        <v>156</v>
+      </c>
       <c r="E161" s="1" t="s">
         <v>564</v>
       </c>
@@ -9188,6 +10312,9 @@
       </c>
     </row>
     <row r="163" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A163" t="s">
+        <v>156</v>
+      </c>
       <c r="E163" s="1" t="s">
         <v>319</v>
       </c>
@@ -9199,6 +10326,9 @@
       </c>
     </row>
     <row r="164" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A164" t="s">
+        <v>156</v>
+      </c>
       <c r="E164" s="1" t="s">
         <v>320</v>
       </c>
@@ -9210,6 +10340,9 @@
       </c>
     </row>
     <row r="165" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A165" t="s">
+        <v>156</v>
+      </c>
       <c r="E165" s="1" t="s">
         <v>323</v>
       </c>
@@ -9221,6 +10354,9 @@
       </c>
     </row>
     <row r="166" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A166" t="s">
+        <v>156</v>
+      </c>
       <c r="E166" s="1" t="s">
         <v>325</v>
       </c>
@@ -9232,6 +10368,9 @@
       </c>
     </row>
     <row r="167" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A167" t="s">
+        <v>156</v>
+      </c>
       <c r="E167" s="1" t="s">
         <v>326</v>
       </c>
@@ -9243,6 +10382,9 @@
       </c>
     </row>
     <row r="168" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A168" t="s">
+        <v>156</v>
+      </c>
       <c r="E168" s="1" t="s">
         <v>329</v>
       </c>
@@ -9254,6 +10396,9 @@
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A169" t="s">
+        <v>156</v>
+      </c>
       <c r="E169" s="1" t="s">
         <v>331</v>
       </c>
@@ -9265,6 +10410,9 @@
       </c>
     </row>
     <row r="170" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A170" t="s">
+        <v>156</v>
+      </c>
       <c r="E170" s="1" t="s">
         <v>333</v>
       </c>
@@ -9276,6 +10424,9 @@
       </c>
     </row>
     <row r="171" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A171" t="s">
+        <v>156</v>
+      </c>
       <c r="E171" s="1" t="s">
         <v>334</v>
       </c>
@@ -9287,6 +10438,9 @@
       </c>
     </row>
     <row r="172" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A172" t="s">
+        <v>156</v>
+      </c>
       <c r="E172" s="1" t="s">
         <v>335</v>
       </c>
@@ -9298,6 +10452,9 @@
       </c>
     </row>
     <row r="173" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A173" t="s">
+        <v>156</v>
+      </c>
       <c r="E173" s="1" t="s">
         <v>336</v>
       </c>
@@ -9332,6 +10489,9 @@
       </c>
     </row>
     <row r="175" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A175" t="s">
+        <v>156</v>
+      </c>
       <c r="E175" s="1" t="s">
         <v>350</v>
       </c>
@@ -9343,6 +10503,9 @@
       </c>
     </row>
     <row r="176" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A176" t="s">
+        <v>156</v>
+      </c>
       <c r="E176" s="1" t="s">
         <v>343</v>
       </c>
@@ -9354,6 +10517,9 @@
       </c>
     </row>
     <row r="177" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A177" t="s">
+        <v>156</v>
+      </c>
       <c r="E177" s="1" t="s">
         <v>348</v>
       </c>
@@ -9365,6 +10531,9 @@
       </c>
     </row>
     <row r="178" spans="1:7" ht="156.6" x14ac:dyDescent="0.4">
+      <c r="A178" t="s">
+        <v>156</v>
+      </c>
       <c r="E178" s="1" t="s">
         <v>349</v>
       </c>
@@ -9376,6 +10545,9 @@
       </c>
     </row>
     <row r="179" spans="1:7" ht="139.19999999999999" x14ac:dyDescent="0.4">
+      <c r="A179" t="s">
+        <v>156</v>
+      </c>
       <c r="E179" s="1" t="s">
         <v>344</v>
       </c>
@@ -9387,6 +10559,9 @@
       </c>
     </row>
     <row r="180" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A180" t="s">
+        <v>156</v>
+      </c>
       <c r="E180" s="1" t="s">
         <v>345</v>
       </c>
@@ -9398,6 +10573,9 @@
       </c>
     </row>
     <row r="181" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A181" t="s">
+        <v>156</v>
+      </c>
       <c r="E181" s="1" t="s">
         <v>346</v>
       </c>
@@ -9409,6 +10587,9 @@
       </c>
     </row>
     <row r="182" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A182" t="s">
+        <v>156</v>
+      </c>
       <c r="E182" s="1" t="s">
         <v>347</v>
       </c>
@@ -9420,6 +10601,9 @@
       </c>
     </row>
     <row r="183" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A183" t="s">
+        <v>156</v>
+      </c>
       <c r="E183" s="1" t="s">
         <v>351</v>
       </c>
@@ -9431,6 +10615,9 @@
       </c>
     </row>
     <row r="184" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A184" t="s">
+        <v>156</v>
+      </c>
       <c r="E184" s="1" t="s">
         <v>352</v>
       </c>
@@ -9442,6 +10629,9 @@
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A185" t="s">
+        <v>156</v>
+      </c>
       <c r="E185" s="1" t="s">
         <v>353</v>
       </c>
@@ -9453,6 +10643,9 @@
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A186" t="s">
+        <v>156</v>
+      </c>
       <c r="E186" s="1" t="s">
         <v>354</v>
       </c>
@@ -9464,6 +10657,9 @@
       </c>
     </row>
     <row r="187" spans="1:7" ht="34.200000000000003" x14ac:dyDescent="0.4">
+      <c r="A187" t="s">
+        <v>156</v>
+      </c>
       <c r="E187" s="1" t="s">
         <v>355</v>
       </c>
@@ -9475,6 +10671,9 @@
       </c>
     </row>
     <row r="188" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A188" t="s">
+        <v>156</v>
+      </c>
       <c r="E188" s="1" t="s">
         <v>356</v>
       </c>
@@ -9486,6 +10685,9 @@
       </c>
     </row>
     <row r="189" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A189" t="s">
+        <v>156</v>
+      </c>
       <c r="E189" s="1" t="s">
         <v>357</v>
       </c>
@@ -9520,6 +10722,9 @@
       </c>
     </row>
     <row r="191" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A191" t="s">
+        <v>156</v>
+      </c>
       <c r="E191" s="1" t="s">
         <v>571</v>
       </c>
@@ -9531,6 +10736,9 @@
       </c>
     </row>
     <row r="192" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A192" t="s">
+        <v>156</v>
+      </c>
       <c r="E192" s="1" t="s">
         <v>572</v>
       </c>
@@ -9542,6 +10750,9 @@
       </c>
     </row>
     <row r="193" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A193" t="s">
+        <v>156</v>
+      </c>
       <c r="E193" s="1" t="s">
         <v>575</v>
       </c>
@@ -9553,6 +10764,9 @@
       </c>
     </row>
     <row r="194" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A194" t="s">
+        <v>156</v>
+      </c>
       <c r="E194" s="1" t="s">
         <v>573</v>
       </c>
@@ -9587,6 +10801,9 @@
       </c>
     </row>
     <row r="196" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A196" t="s">
+        <v>156</v>
+      </c>
       <c r="E196" s="1" t="s">
         <v>581</v>
       </c>
@@ -9598,6 +10815,9 @@
       </c>
     </row>
     <row r="197" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A197" t="s">
+        <v>156</v>
+      </c>
       <c r="E197" s="1" t="s">
         <v>582</v>
       </c>
@@ -9609,6 +10829,9 @@
       </c>
     </row>
     <row r="198" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A198" t="s">
+        <v>156</v>
+      </c>
       <c r="E198" s="1" t="s">
         <v>583</v>
       </c>
@@ -9620,6 +10843,9 @@
       </c>
     </row>
     <row r="199" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A199" t="s">
+        <v>156</v>
+      </c>
       <c r="E199" s="1" t="s">
         <v>584</v>
       </c>
@@ -9654,6 +10880,9 @@
       </c>
     </row>
     <row r="201" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A201" t="s">
+        <v>156</v>
+      </c>
       <c r="E201" s="1" t="s">
         <v>591</v>
       </c>
@@ -9665,6 +10894,9 @@
       </c>
     </row>
     <row r="202" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A202" t="s">
+        <v>156</v>
+      </c>
       <c r="E202" s="1" t="s">
         <v>592</v>
       </c>
@@ -9676,6 +10908,9 @@
       </c>
     </row>
     <row r="203" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A203" t="s">
+        <v>156</v>
+      </c>
       <c r="E203" s="1" t="s">
         <v>593</v>
       </c>
@@ -9687,6 +10922,9 @@
       </c>
     </row>
     <row r="204" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A204" t="s">
+        <v>156</v>
+      </c>
       <c r="E204" s="1" t="s">
         <v>594</v>
       </c>
@@ -9721,6 +10959,9 @@
       </c>
     </row>
     <row r="206" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A206" t="s">
+        <v>156</v>
+      </c>
       <c r="E206" s="1" t="s">
         <v>601</v>
       </c>
@@ -9732,6 +10973,9 @@
       </c>
     </row>
     <row r="207" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A207" t="s">
+        <v>156</v>
+      </c>
       <c r="E207" s="1" t="s">
         <v>602</v>
       </c>
@@ -9743,6 +10987,9 @@
       </c>
     </row>
     <row r="208" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A208" t="s">
+        <v>156</v>
+      </c>
       <c r="E208" s="1" t="s">
         <v>603</v>
       </c>
@@ -9754,6 +11001,9 @@
       </c>
     </row>
     <row r="209" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A209" t="s">
+        <v>156</v>
+      </c>
       <c r="E209" s="1" t="s">
         <v>604</v>
       </c>
@@ -9788,6 +11038,9 @@
       </c>
     </row>
     <row r="211" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A211" t="s">
+        <v>156</v>
+      </c>
       <c r="E211" s="1" t="s">
         <v>611</v>
       </c>
@@ -9799,6 +11052,9 @@
       </c>
     </row>
     <row r="212" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A212" t="s">
+        <v>156</v>
+      </c>
       <c r="E212" s="1" t="s">
         <v>612</v>
       </c>
@@ -9810,6 +11066,9 @@
       </c>
     </row>
     <row r="213" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A213" t="s">
+        <v>156</v>
+      </c>
       <c r="E213" s="1" t="s">
         <v>613</v>
       </c>
@@ -9821,6 +11080,9 @@
       </c>
     </row>
     <row r="214" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A214" t="s">
+        <v>156</v>
+      </c>
       <c r="E214" s="1" t="s">
         <v>614</v>
       </c>
@@ -9855,6 +11117,9 @@
       </c>
     </row>
     <row r="216" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A216" t="s">
+        <v>156</v>
+      </c>
       <c r="E216" s="1" t="s">
         <v>622</v>
       </c>
@@ -9866,6 +11131,9 @@
       </c>
     </row>
     <row r="217" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A217" t="s">
+        <v>156</v>
+      </c>
       <c r="E217" s="1" t="s">
         <v>623</v>
       </c>
@@ -9877,6 +11145,9 @@
       </c>
     </row>
     <row r="218" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A218" t="s">
+        <v>156</v>
+      </c>
       <c r="E218" s="1" t="s">
         <v>624</v>
       </c>
@@ -9888,6 +11159,9 @@
       </c>
     </row>
     <row r="219" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A219" t="s">
+        <v>156</v>
+      </c>
       <c r="E219" s="1" t="s">
         <v>625</v>
       </c>
@@ -9922,6 +11196,9 @@
       </c>
     </row>
     <row r="221" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A221" t="s">
+        <v>156</v>
+      </c>
       <c r="E221" s="1" t="s">
         <v>631</v>
       </c>
@@ -9933,6 +11210,9 @@
       </c>
     </row>
     <row r="222" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A222" t="s">
+        <v>156</v>
+      </c>
       <c r="E222" s="1" t="s">
         <v>632</v>
       </c>
@@ -9944,6 +11224,9 @@
       </c>
     </row>
     <row r="223" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A223" t="s">
+        <v>156</v>
+      </c>
       <c r="E223" s="1" t="s">
         <v>633</v>
       </c>
@@ -9955,6 +11238,9 @@
       </c>
     </row>
     <row r="224" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A224" t="s">
+        <v>156</v>
+      </c>
       <c r="E224" s="1" t="s">
         <v>634</v>
       </c>
@@ -9989,6 +11275,9 @@
       </c>
     </row>
     <row r="226" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A226" t="s">
+        <v>156</v>
+      </c>
       <c r="E226" s="1" t="s">
         <v>641</v>
       </c>
@@ -10000,6 +11289,9 @@
       </c>
     </row>
     <row r="227" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A227" t="s">
+        <v>156</v>
+      </c>
       <c r="E227" s="1" t="s">
         <v>642</v>
       </c>
@@ -10011,6 +11303,9 @@
       </c>
     </row>
     <row r="228" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A228" t="s">
+        <v>156</v>
+      </c>
       <c r="E228" s="1" t="s">
         <v>643</v>
       </c>
@@ -10022,6 +11317,9 @@
       </c>
     </row>
     <row r="229" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A229" t="s">
+        <v>156</v>
+      </c>
       <c r="E229" s="1" t="s">
         <v>644</v>
       </c>
@@ -10056,6 +11354,9 @@
       </c>
     </row>
     <row r="231" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A231" t="s">
+        <v>156</v>
+      </c>
       <c r="E231" s="1" t="s">
         <v>651</v>
       </c>
@@ -10067,6 +11368,9 @@
       </c>
     </row>
     <row r="232" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A232" t="s">
+        <v>156</v>
+      </c>
       <c r="E232" s="1" t="s">
         <v>652</v>
       </c>
@@ -10078,6 +11382,9 @@
       </c>
     </row>
     <row r="233" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A233" t="s">
+        <v>156</v>
+      </c>
       <c r="E233" s="1" t="s">
         <v>653</v>
       </c>
@@ -10089,6 +11396,9 @@
       </c>
     </row>
     <row r="234" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A234" t="s">
+        <v>156</v>
+      </c>
       <c r="E234" s="1" t="s">
         <v>654</v>
       </c>
@@ -10123,6 +11433,9 @@
       </c>
     </row>
     <row r="236" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A236" t="s">
+        <v>156</v>
+      </c>
       <c r="E236" s="1" t="s">
         <v>661</v>
       </c>
@@ -10134,6 +11447,9 @@
       </c>
     </row>
     <row r="237" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A237" t="s">
+        <v>156</v>
+      </c>
       <c r="E237" s="1" t="s">
         <v>662</v>
       </c>
@@ -10145,6 +11461,9 @@
       </c>
     </row>
     <row r="238" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A238" t="s">
+        <v>156</v>
+      </c>
       <c r="E238" s="1" t="s">
         <v>664</v>
       </c>
@@ -10156,6 +11475,9 @@
       </c>
     </row>
     <row r="239" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A239" t="s">
+        <v>156</v>
+      </c>
       <c r="E239" s="1" t="s">
         <v>665</v>
       </c>
@@ -10190,6 +11512,9 @@
       </c>
     </row>
     <row r="241" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A241" t="s">
+        <v>156</v>
+      </c>
       <c r="E241" s="1" t="s">
         <v>680</v>
       </c>
@@ -10201,6 +11526,9 @@
       </c>
     </row>
     <row r="242" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A242" t="s">
+        <v>156</v>
+      </c>
       <c r="E242" s="1" t="s">
         <v>673</v>
       </c>
@@ -10212,6 +11540,9 @@
       </c>
     </row>
     <row r="243" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A243" t="s">
+        <v>156</v>
+      </c>
       <c r="E243" s="1" t="s">
         <v>674</v>
       </c>
@@ -10223,6 +11554,9 @@
       </c>
     </row>
     <row r="244" spans="1:7" ht="174" x14ac:dyDescent="0.4">
+      <c r="A244" t="s">
+        <v>156</v>
+      </c>
       <c r="E244" s="1" t="s">
         <v>681</v>
       </c>
@@ -10257,6 +11591,9 @@
       </c>
     </row>
     <row r="246" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A246" t="s">
+        <v>156</v>
+      </c>
       <c r="E246" s="1" t="s">
         <v>683</v>
       </c>
@@ -10268,6 +11605,9 @@
       </c>
     </row>
     <row r="247" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A247" t="s">
+        <v>156</v>
+      </c>
       <c r="E247" s="1" t="s">
         <v>684</v>
       </c>
@@ -10279,6 +11619,9 @@
       </c>
     </row>
     <row r="248" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A248" t="s">
+        <v>156</v>
+      </c>
       <c r="E248" s="1" t="s">
         <v>685</v>
       </c>
@@ -10290,6 +11633,9 @@
       </c>
     </row>
     <row r="249" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A249" t="s">
+        <v>156</v>
+      </c>
       <c r="E249" s="1" t="s">
         <v>686</v>
       </c>
@@ -10324,6 +11670,9 @@
       </c>
     </row>
     <row r="251" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A251" t="s">
+        <v>156</v>
+      </c>
       <c r="E251" s="1" t="s">
         <v>693</v>
       </c>
@@ -10335,6 +11684,9 @@
       </c>
     </row>
     <row r="252" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A252" t="s">
+        <v>156</v>
+      </c>
       <c r="E252" s="1" t="s">
         <v>694</v>
       </c>
@@ -10346,6 +11698,9 @@
       </c>
     </row>
     <row r="253" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A253" t="s">
+        <v>156</v>
+      </c>
       <c r="E253" s="1" t="s">
         <v>695</v>
       </c>
@@ -10357,6 +11712,9 @@
       </c>
     </row>
     <row r="254" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A254" t="s">
+        <v>156</v>
+      </c>
       <c r="E254" s="1" t="s">
         <v>696</v>
       </c>
@@ -10391,6 +11749,9 @@
       </c>
     </row>
     <row r="256" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A256" t="s">
+        <v>156</v>
+      </c>
       <c r="E256" s="1" t="s">
         <v>703</v>
       </c>
@@ -10402,6 +11763,9 @@
       </c>
     </row>
     <row r="257" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A257" t="s">
+        <v>156</v>
+      </c>
       <c r="E257" s="1" t="s">
         <v>704</v>
       </c>
@@ -10413,6 +11777,9 @@
       </c>
     </row>
     <row r="258" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A258" t="s">
+        <v>156</v>
+      </c>
       <c r="E258" s="1" t="s">
         <v>705</v>
       </c>
@@ -10424,6 +11791,9 @@
       </c>
     </row>
     <row r="259" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A259" t="s">
+        <v>156</v>
+      </c>
       <c r="E259" s="1" t="s">
         <v>706</v>
       </c>
@@ -10458,6 +11828,9 @@
       </c>
     </row>
     <row r="261" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A261" t="s">
+        <v>156</v>
+      </c>
       <c r="E261" s="1" t="s">
         <v>713</v>
       </c>
@@ -10469,6 +11842,9 @@
       </c>
     </row>
     <row r="262" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A262" t="s">
+        <v>156</v>
+      </c>
       <c r="E262" s="1" t="s">
         <v>714</v>
       </c>
@@ -10480,6 +11856,9 @@
       </c>
     </row>
     <row r="263" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A263" t="s">
+        <v>156</v>
+      </c>
       <c r="E263" s="1" t="s">
         <v>715</v>
       </c>
@@ -10491,6 +11870,9 @@
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A264" t="s">
+        <v>156</v>
+      </c>
       <c r="E264" s="1" t="s">
         <v>716</v>
       </c>
@@ -10525,6 +11907,9 @@
       </c>
     </row>
     <row r="266" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A266" t="s">
+        <v>156</v>
+      </c>
       <c r="E266" s="1" t="s">
         <v>723</v>
       </c>
@@ -10536,6 +11921,9 @@
       </c>
     </row>
     <row r="267" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A267" t="s">
+        <v>156</v>
+      </c>
       <c r="E267" s="1" t="s">
         <v>724</v>
       </c>
@@ -10547,6 +11935,9 @@
       </c>
     </row>
     <row r="268" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A268" t="s">
+        <v>156</v>
+      </c>
       <c r="E268" s="1" t="s">
         <v>725</v>
       </c>
@@ -10558,6 +11949,9 @@
       </c>
     </row>
     <row r="269" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A269" t="s">
+        <v>156</v>
+      </c>
       <c r="E269" s="1" t="s">
         <v>726</v>
       </c>
@@ -10592,6 +11986,9 @@
       </c>
     </row>
     <row r="271" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A271" t="s">
+        <v>156</v>
+      </c>
       <c r="E271" s="1" t="s">
         <v>375</v>
       </c>
@@ -10603,6 +12000,9 @@
       </c>
     </row>
     <row r="272" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A272" t="s">
+        <v>156</v>
+      </c>
       <c r="E272" s="1" t="s">
         <v>376</v>
       </c>
@@ -10614,6 +12014,9 @@
       </c>
     </row>
     <row r="273" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A273" t="s">
+        <v>156</v>
+      </c>
       <c r="E273" s="1" t="s">
         <v>379</v>
       </c>
@@ -10625,6 +12028,9 @@
       </c>
     </row>
     <row r="274" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A274" t="s">
+        <v>156</v>
+      </c>
       <c r="E274" s="1" t="s">
         <v>381</v>
       </c>
@@ -10636,6 +12042,9 @@
       </c>
     </row>
     <row r="275" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A275" t="s">
+        <v>156</v>
+      </c>
       <c r="E275" s="1" t="s">
         <v>383</v>
       </c>
@@ -10647,6 +12056,9 @@
       </c>
     </row>
     <row r="276" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A276" t="s">
+        <v>156</v>
+      </c>
       <c r="E276" s="1" t="s">
         <v>384</v>
       </c>
@@ -10658,6 +12070,9 @@
       </c>
     </row>
     <row r="277" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A277" t="s">
+        <v>156</v>
+      </c>
       <c r="E277" s="1" t="s">
         <v>387</v>
       </c>
@@ -10669,6 +12084,9 @@
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A278" t="s">
+        <v>156</v>
+      </c>
       <c r="E278" s="1" t="s">
         <v>389</v>
       </c>
@@ -10703,6 +12121,9 @@
       </c>
     </row>
     <row r="280" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A280" t="s">
+        <v>156</v>
+      </c>
       <c r="E280" s="1" t="s">
         <v>393</v>
       </c>
@@ -10714,6 +12135,9 @@
       </c>
     </row>
     <row r="281" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A281" t="s">
+        <v>156</v>
+      </c>
       <c r="E281" s="1" t="s">
         <v>394</v>
       </c>
@@ -10725,6 +12149,9 @@
       </c>
     </row>
     <row r="282" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A282" t="s">
+        <v>156</v>
+      </c>
       <c r="E282" s="1" t="s">
         <v>395</v>
       </c>
@@ -10736,6 +12163,9 @@
       </c>
     </row>
     <row r="283" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A283" t="s">
+        <v>156</v>
+      </c>
       <c r="E283" s="1" t="s">
         <v>396</v>
       </c>
@@ -10747,6 +12177,9 @@
       </c>
     </row>
     <row r="284" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A284" t="s">
+        <v>156</v>
+      </c>
       <c r="E284" s="1" t="s">
         <v>401</v>
       </c>
@@ -10758,6 +12191,9 @@
       </c>
     </row>
     <row r="285" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A285" t="s">
+        <v>156</v>
+      </c>
       <c r="E285" s="1" t="s">
         <v>403</v>
       </c>
@@ -10769,6 +12205,9 @@
       </c>
     </row>
     <row r="286" spans="1:7" ht="139.19999999999999" x14ac:dyDescent="0.4">
+      <c r="A286" t="s">
+        <v>156</v>
+      </c>
       <c r="E286" s="1" t="s">
         <v>404</v>
       </c>
@@ -10780,6 +12219,9 @@
       </c>
     </row>
     <row r="287" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A287" t="s">
+        <v>156</v>
+      </c>
       <c r="E287" s="1" t="s">
         <v>405</v>
       </c>
@@ -10791,6 +12233,9 @@
       </c>
     </row>
     <row r="288" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A288" t="s">
+        <v>156</v>
+      </c>
       <c r="E288" s="1" t="s">
         <v>406</v>
       </c>
@@ -10801,7 +12246,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="289" spans="1:4" ht="104.4" x14ac:dyDescent="0.4">
+    <row r="289" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A289" t="s">
         <v>156</v>
       </c>
@@ -10814,89 +12259,572 @@
       <c r="D289" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="290" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="E289" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="F289" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="G289">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A290" t="s">
         <v>156</v>
       </c>
-      <c r="B290" s="1" t="s">
+      <c r="E290" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="F290" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="G290">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A291" t="s">
+        <v>156</v>
+      </c>
+      <c r="E291" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="F291" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="G291">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A292" t="s">
+        <v>156</v>
+      </c>
+      <c r="E292" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="F292" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="G292">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A293" t="s">
+        <v>156</v>
+      </c>
+      <c r="E293" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="F293" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="G293">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A294" t="s">
+        <v>156</v>
+      </c>
+      <c r="B294" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C290" s="1" t="s">
+      <c r="C294" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="D290" s="1" t="s">
+      <c r="D294" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="291" spans="1:4" ht="104.4" x14ac:dyDescent="0.4">
-      <c r="A291" t="s">
-        <v>156</v>
-      </c>
-      <c r="B291" s="1" t="s">
+      <c r="E294" s="1" t="s">
+        <v>742</v>
+      </c>
+      <c r="F294" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="G294">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A295" t="s">
+        <v>156</v>
+      </c>
+      <c r="E295" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="F295" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="G295">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A296" t="s">
+        <v>156</v>
+      </c>
+      <c r="E296" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="F296" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="G296">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A297" t="s">
+        <v>156</v>
+      </c>
+      <c r="E297" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="F297" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="G297">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A298" t="s">
+        <v>156</v>
+      </c>
+      <c r="E298" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="F298" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="G298">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A299" t="s">
+        <v>156</v>
+      </c>
+      <c r="B299" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="C291" s="1" t="s">
+      <c r="C299" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D291" s="1" t="s">
+      <c r="D299" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="292" spans="1:4" ht="87" x14ac:dyDescent="0.4">
-      <c r="A292" t="s">
-        <v>156</v>
-      </c>
-      <c r="B292" s="1" t="s">
+      <c r="E299" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="F299" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="G299">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A300" t="s">
+        <v>156</v>
+      </c>
+      <c r="E300" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="F300" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="G300">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A301" t="s">
+        <v>156</v>
+      </c>
+      <c r="E301" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="F301" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="G301">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A302" t="s">
+        <v>156</v>
+      </c>
+      <c r="E302" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="F302" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="G302">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A303" t="s">
+        <v>156</v>
+      </c>
+      <c r="E303" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="F303" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="G303">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A304" t="s">
+        <v>156</v>
+      </c>
+      <c r="E304" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="F304" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="G304">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A305" t="s">
+        <v>156</v>
+      </c>
+      <c r="E305" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="F305" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="G305">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A306" t="s">
+        <v>156</v>
+      </c>
+      <c r="B306" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C292" s="1" t="s">
+      <c r="C306" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D292" s="1" t="s">
+      <c r="D306" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="293" spans="1:4" ht="87" x14ac:dyDescent="0.4">
-      <c r="A293" t="s">
-        <v>156</v>
-      </c>
-      <c r="B293" s="1" t="s">
+      <c r="E306" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="F306" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="G306">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A307" t="s">
+        <v>156</v>
+      </c>
+      <c r="E307" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="F307" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="G307">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A308" t="s">
+        <v>156</v>
+      </c>
+      <c r="E308" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="F308" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="G308">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A309" t="s">
+        <v>156</v>
+      </c>
+      <c r="E309" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="F309" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="G309">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A310" t="s">
+        <v>156</v>
+      </c>
+      <c r="E310" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="F310" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="G310">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A311" t="s">
+        <v>156</v>
+      </c>
+      <c r="B311" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C293" s="1" t="s">
+      <c r="C311" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D293" s="1" t="s">
+      <c r="D311" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="294" spans="1:4" ht="52.2" x14ac:dyDescent="0.4">
-      <c r="A294" t="s">
-        <v>156</v>
-      </c>
-      <c r="B294" s="1" t="s">
+      <c r="E311" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="F311" s="1" t="s">
+        <v>781</v>
+      </c>
+      <c r="G311">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A312" t="s">
+        <v>156</v>
+      </c>
+      <c r="E312" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="F312" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="G312">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A313" t="s">
+        <v>156</v>
+      </c>
+      <c r="E313" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="F313" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="G313">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A314" t="s">
+        <v>156</v>
+      </c>
+      <c r="E314" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="F314" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="G314">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A315" t="s">
+        <v>156</v>
+      </c>
+      <c r="E315" s="1" t="s">
+        <v>779</v>
+      </c>
+      <c r="F315" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="G315">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A316" t="s">
+        <v>156</v>
+      </c>
+      <c r="B316" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C294" s="1" t="s">
+      <c r="C316" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D294" s="1" t="s">
+      <c r="D316" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="295" spans="1:4" ht="121.8" x14ac:dyDescent="0.4">
-      <c r="A295" t="s">
-        <v>156</v>
-      </c>
-      <c r="B295" s="1" t="s">
+      <c r="E316" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="F316" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="G316">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A317" t="s">
+        <v>156</v>
+      </c>
+      <c r="E317" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="F317" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="G317">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A318" t="s">
+        <v>156</v>
+      </c>
+      <c r="E318" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="F318" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="G318">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A319" t="s">
+        <v>156</v>
+      </c>
+      <c r="E319" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="F319" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="G319">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A320" t="s">
+        <v>156</v>
+      </c>
+      <c r="E320" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="F320" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="G320">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A321" t="s">
+        <v>156</v>
+      </c>
+      <c r="B321" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C295" s="1" t="s">
+      <c r="C321" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D295" s="1" t="s">
+      <c r="D321" s="1" t="s">
         <v>153</v>
+      </c>
+      <c r="E321" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="F321" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="G321">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A322" t="s">
+        <v>156</v>
+      </c>
+      <c r="E322" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="F322" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="G322">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A323" t="s">
+        <v>156</v>
+      </c>
+      <c r="E323" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="F323" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="G323">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A324" t="s">
+        <v>156</v>
+      </c>
+      <c r="E324" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="F324" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="G324">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A325" t="s">
+        <v>156</v>
+      </c>
+      <c r="E325" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="F325" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="G325">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ADD: ML quiz valid dataset (1)
</commit_message>
<xml_diff>
--- a/2025_07_02_OhLoRA_ML_Tutor/ai_quiz/dataset/all_train_and_test_data.xlsx
+++ b/2025_07_02_OhLoRA_ML_Tutor/ai_quiz/dataset/all_train_and_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA56D8B2-7E40-4134-B488-C9DF9F04D19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB91AE8-C31D-4992-9EFB-04601338525D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{07338742-8F51-42F9-A75F-1FCFBE7C4D0C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="879">
   <si>
     <t>quiz</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -7400,6 +7400,298 @@
       </rPr>
       <t>👍👍</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>valid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코사인 유사도는 벡터의 방향을 가지고 판단하는 유사도이다. 벡터 방향이 일치할수록 +1.0, 반대 방향일수록 -1.0에 가까운 값을 갖는다. 코사인 유사도는 S-BERT, 추천 시스템 등에서 사용한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>벡터의 유사도를 판단하기 위해 사용한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정확도는 전체 예측 중 정답의 개수이고, 재현율은 실제로 참인 개수 중 모델의 예측이 참인 개수의 비율을 의미한다. 정밀도는 재현율과는 다르게 모델이 참으로 예측한 것 중 실제 참인 것의 비율이고, F1 Score 는 정밀도와 재현율의 조화 평균이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F1 Score = 2 * 정밀도 * 재현율 / (정밀도 + 재현율)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IoU 는 예측이 True 인 집합과 실제 값이 True 인 집합을 고려했을 때, 그 (교집합의 원소의 개수) / (합집합의 원소의 개수) 이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IoU 는 교집합 / 합집합의 크기, DICE score 는 음… 잘 모르겠다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PR-AUC 와 AUC-ROC 는 이진 분류에서 사용하는 성능지표이다. 둘 다 값의 범위는 0~1이고 1에 가까울수록 좋은 성능을 나타낸다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PR-AUC 와 AUC-ROC 는 이진 분류에서 사용하는 성능지표이다. 둘 다 값의 범위는 0~1이고 1에 가까울수록 좋은 성능을 나타낸다. 이 중 PR-AUC는 x축과 y축이 각각 recall, precision 이고, ROC-AUC 는 각각 FP rate 와 TP rate 이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>결측값은 머신러닝 학습 데이터의 데이터셋에서 일부 데이터가 누락된 것이다. 이를 해결하기 위해서 결측값을 채워야 하는데, 평균값, 중앙값, 최빈값, k-NN, 딥러닝 기반 등의 알고리즘이 사용된다. 혹은 모델 자체 알고리즘을 사용하기도 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터에서 어떤 값이 누락된 것이고, 평균값으로 대체한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정규화는 데이터를 일정한 수식을 이용해서 변환하는 것을 통해 전처리하는 방법이다. 머신러닝 모델의 학습 용이성, 표준편차 차이로 인한 각 특징의 학습 불균형을 해결하기 위한 방법이다. 정규와 알고리즘에는 Min-max (최솟값을 0, 최댓값을 1로 mapping 시키는 선형 방법), Z-score (평균과 표준편차를 이용하는 것), 최솟값을 올리고 최댓값을 내려서 모든 데이터를 일정 범위 내로 mapping 시키는 Clipping, 로그 스케일 변환이 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정규화는 데이터의 각 속성별로 평균과 표준편차를 이용하여 표준정규분포로 변환하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이상치는 아웃라이어라고 하며, 데이터셋의 정상적인 범위를 벗어난 값이다. 데이터 시각화 가독성을 해치고, 특정 정규화 방법 (Min-max 등) 에서 Outlier 의 영향으로 데이터 분포가 크게 이상해질 수 있으며, 머신러닝 학습에도 지장이 될 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이상치는 데이터에서 일반적인 분포 범위를 크게 벗어난 아웃라이어를 의미한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PCA는 데이터셋 분산의 보존에 초점을 둔다. T-SNE는 시각화에 초점을 둔다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>t-SNE는 2~3차원으로 데이터를 축소하여 시각화에 용이하도록 하는 방법이다. 즉 PCA와는 다르다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>확률은 확률분포에서 특정 값이 관측될 가능성, 우도는 어떤 관측값이 주어질 때 그 관측값이 어떤 확률분포로부터 발생했을 가능성이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>확률은 확률분포에서 특정 값의 확률이고 우도는 그 반대이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 불균형은 Class 간 데이터 개수가 서로 유의미하게 차이 나는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 불균형은 Class 간 데이터 개수가 서로 유의미하게 차이 나는 것이다. Minority 데이터의 개수를 늘리거나, 데이터 증강을 하거나, 성능 평가 지표를 F1 Score 같은 걸로 바꾸는 방법으로 해결할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>차원의 저주는 학습 데이터의 feature 가 불필요하게 너무 많아져서 오히려 학습에 방해되는 것을 말한다. 학습 속도가 감소하고, OOM이 발생하고, 모델 성능이 감소한다. 해결 방법은 기존 feature 중 일부만 사용하는 것, PCA처럼 차원을 축소하는 것이 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>차원의 저주는 차원이 너무 많아져서 OOM이 발생하는 것으로, PCA로 해결하면 된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>학습할 때 feature 조건을 여러 개 만들고, 그것들 중 class 를 가장 잘 구분할 수 있는 조건을 선택한다. 추론할 때는 맨 위에서 시작해서 그 데이터가 가지고 있는 속성 값에 따라 적절한 분기를 끝까지 선택해 나간다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>분기된 feature 조건이 해당 조건에 의해 분기된 각 분기 안에 속하는 데이터의 불순도 (다양한 정도) 가 최소화되도록 학습한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>앙상블은 여러 개의 모델을 사용해서 예측하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>앙상블은 모델을 하나가 아닌 여러 개 쓰는 것</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>앙상블의 방법에는 Voting, Bagging, Stacking 이 있다. Voting 은 Soft Voting (여러 모델의 예측값의 평균값) 과 Hard Voting (여러 모델의 예측 결과의 다수결) 이 있다. Bagging 은 원본 데이터셋으로부터 랜덤 샘플링한 데이터셋을 여러 개 만들고, 각 데이터셋을 이용하여 모델을 학습시키는 것이다. 그리고 이 학습된 모델들에 의한 예측 결과를 종합한다. 마지막으로 Stacking 은 개별 모델의 예측값이 입력, 실제 데이터 값이 출력인 메타 모델을 학습, 해당 메타 모델의 출력값이 최종 예측값이 되는 형태이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Voting 은 Soft Voting 과 Hard Voting 으로 나뉜다. Voting 은 Soft Voting 과 Hard Voting 으로 나뉜다. Voting 은 Soft Voting 과 Hard Voting 으로 나뉜다. Voting 은 Soft Voting 과 Hard Voting 으로 나뉜다. Voting 은 Soft Voting 과 Hard Voting 으로 나뉜다. Voting 은 Soft Voting 과 Hard Voting 으로 나뉜다. Voting 은 Soft Voting 과 Hard Voting 으로 나뉜다. Voting 은 Soft Voting 과 Hard Voting 으로 나뉜다. Voting 은 Soft Voting 과 Hard Voting 으로 나뉜다. Voting 은 Soft Voting 과 Hard Voting 으로 나뉜다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mean point 를 K 개 먼저 지정하고, 데이터셋에 있는 각 Point 에 대해서 다음을 반복한다. 1. 그 class 를 K개의 점 중 가장 가까운 점의 class 로 할당. 2. 각각의 K 개의 mean point 를 이들 point 중 해당 class에 속하는 모든 점의 평균으로 갱신. 언제까지? 수렴할 때까지.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>K-means Clustering 은 먼저 랜덤한 mean point 를 K개 지정해서 초기화한다. 그런 다음 어떤 과정을 수렴할 때까지 계속 반복한다. 그런데 그 과정이 뭐였지? 진까 까먹었는데. 로라야 도와줘!!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지도학습과 비지도학습은 각각 사용자나 데이터셋의 지도를 가지고, 사용자의 지도 없이 학습하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지도학습은 입력과 출력을 모두 사용하는 학습 방식으로 모델이 어떤 입력에 대해 목적한 출력을 하도록 학습시키는 것이다. 비지도학습은 출력 없이 입력만을 모델이 알잘딱깔센하게 학습하도록 하는 방법이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조건부 확률 이론인 베이즈 정리 기반으로 작동한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>베이즈 정리 기반으로, 각 Class 별로 (전체 데이터셋에서의 해당 Class 의 비율) x 각 속성별로 (해당 Class 에 속한 데이터 중 속성 값이 새로 입력된 데이터와 일치하는 것의 비율) 의 전체 곱을 구하고, 이 전체 곱이 가장 큰 Class 로 최종 예측한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아 이거 PCA가 진짜 뭐였지</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터셋의 분산을 최대한 보존하도록 동작한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decision Tree 를 발전시킨 Random Forest 는 Decision Tree 를 아주 많이 만드는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Decision Tree 를 아주 많이 만들고 그것들의 예측 결과를 합쳐서 앙상블 시키는 것이다. 즉 Decision Tree 를 발전시킨 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2개의 Class 간의 구분선을 만들 때 각 Class 간의 거리가 최대가 되는 구분선을 찾는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2개의 Class 가 있을 때 사용하며, 이들 간 마진이 최대가 되는 구분선을 찾는 것이 핵심 아이디어이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>K-fold Validation 만으로 어차피 충분하므로 Stratified 까지는 굳이 안 해도 된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 불균형을 해소하기 위한 방법으로, Stratified K-fold Validation 을 사용하면 데이터 개수가 적은 Class 가 표본 부족으로 각 fold 에 고르지 않게 분포되는 이슈가 있다. 즉 이를 해결하기 위한 방법이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>train data 보다 과거의 데이터가 valid data 에 포함되면 학습에 지장을 줄 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>train data 보다 과거의 데이터가 valid data 에 포함되면 학습에 지장을 줄 수 있다. 따라서 이를 해결하기 위해 train data 는 항상 valid data 의 과거 시점 데이터로만 구성한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하이퍼파라미터는 딥러닝 모델의 신경망의 파라미터를 의미한다. 하이퍼파라미터 최적화는 이 딥러닝 모델의 파라미터를 각종 최적화 기술 (Optimizer, Regularization, Dropout, 기타등등) 을 이용하여 최적의 상태로 학습시켜서 Loss Function 의 값을 최대한 줄이는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하이퍼파라미터는 모델의 학습 과정 자체를 결정하는 설정값으로, 그 최적화 방법으로는 search space 에서 바둑판 격자 모양으로 탐색하는 Grid Search, 랜덤하게 탐색하는 Random Search가 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valid Dataset 이 필요한 이유는 Test Dataset 만으로 부족한 뭔가를 채우기 위해서이다. 근데 그게 뭔지 솔직히 모르겠다. ㅋㅋㅋ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Train 데이터셋의 성능 평가를 Test Dataset 으로만 하면 하이퍼파라미터 같은 것을 개선하거나 모델 구조를 바꾸거나 다른 모델을 사용할 때 최종 테스트용 데이터셋을 사용하므로 추가적인 테스트 데이터셋이 없어지게 된다. 이를 방지하기 위해 검증용 데이터셋인 Valid Dataset 을 사용한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터 순서마저 모델이 학습하거나 데이터 순서로 인해 모델의 학습의 Loss Function 등에 영향을 받을 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어차피 다들 PyTorch 할때 train dataset 은 섞던데 그냥 섞는게 당연한 거 아닌가? 잘 모르겠다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Valid Dataset 에 대한 Loss 가 일정 epoch 동안 최저 기록을 갱신하지 않으면 학습을 중단하는 것이며, overfitting 방지를 위한 조정책으로 반드시 필요하다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오버피팅을 막기 위해 Valid Dataset Loss 가 더 이상 떨어지지 않으면 학습을 종료하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지식 증류는 어떤 데이터셋으로 사전학습 (Pre-train) 된 모델을 해당 모델을 적용 가능한 다른 데이터셋 또는 다른 task 의 데이터셋으로 추가 학습 (Fine-Tuning) 시키는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지식 증류는 거대한 모델의 지식을 보다 작은 모델로 전수하여 모델 경량화를 달성하는 것이다. Offline, Online, Self Distillation 으로 나뉜다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>학습률을 시간이 지남에 따라 조정하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>학습률을 시간이 지남에 따라 조정하는 알고리즘으로, 학습 초반에는 빠르게 학습하고, 중반 이후에는 안정적으로 수렴할 수 있도록 하는 역할을 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그냥 롤러코스터처럼 학습률을 움직이는 것이 재미있기 때문이다. 딥러닝 모델도 학습에 재미를 느껴야지 원활한 학습이 가능하기 때문이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>local minima 를 벗어나게 하려고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loss, Cost, Objective Function 셋 다 딥러닝에서 모델을 목적에 맞게 최적화하기 위해 페널티 느낌으로 사용하는 함수이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Objective Function 은 딥러닝 모델의 학습 방향을 목적에 맞게 결정하기 위한 함수이다. 이 중 최소화해야 하는 함수는 Loss Function 또는 Cost Function 이라고 하는데, Loss Function 은 개별 샘플, Cost Function 은 전체 데이터 관점에서의 함수이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multi Class: Categorical Cross Entropy, Multi-Label : BCE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multi Class: Categorical Cross Entropy, Multi-Label : BCE (각 Class 별로)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSE = Mean Squared Error, MAE = Mean Absolute Error, 그리고 RMSE는 MSE를 제곱근 처리한 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MSE = Mean Squared Error, MAE = Mean Absolute Error, 그리고 RMSE는 Root Mean Squared Error 로 MSE를 제곱근 처리한 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아 Optimizer 다 까먹었는데 다시 한번 복습 좀 해야겠다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AdamW 는 weight decay 를 적용한 decoupled weight decay 를 사용한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weight Decay 는 가중치 감쇠라고도 하며 모델의 이전 가중치의 크기에 일정 비율을 곱해서 이를 감소시키는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Weight Decay 는 가중치 감쇠라고도 하며 모델의 이전 가중치의 크기에 일정 비율을 곱해서 이를 감소시키는 것이다. Weight Decay 가 사용되는 곳은 AdamW 이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>딥러닝 모델이 필요 이상으로 학습하게 되면 valid 나 test 데이터셋에 대해서 오차가 오히려 점점 늘어나게 되는데 이것을 Overfitting 이라고 한다. Dropout 을 충실히 적용하면 해결할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>드롭아웃을 적용해서 해결한다. 아니면 Batch Normalization, 데이터 증강, Early Stopping 으로 해결할 수도 있고, 모델 구조를 보다 간단하게 만들어서 해결할 수도 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>드롭아웃은 신경망에서 각 뉴런을 일정 확률로 독립적으로 제거하는 것을 말한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>드롭아웃은 신경망에서 각 뉴런을 일정 확률로 독립적으로 제거하는 것을 말한다. 오버피팅을 막는다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7783,10 +8075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF56922-B03A-4496-8414-3644939C6218}">
-  <dimension ref="A1:G325"/>
+  <dimension ref="A1:G428"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A392" workbookViewId="0">
+      <selection activeCell="E398" sqref="E398"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -12827,6 +13119,1241 @@
         <v>1</v>
       </c>
     </row>
+    <row r="326" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A326" t="s">
+        <v>806</v>
+      </c>
+      <c r="B326" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D326" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E326" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="G326">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A327" t="s">
+        <v>806</v>
+      </c>
+      <c r="E327" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="G327">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A328" t="s">
+        <v>806</v>
+      </c>
+      <c r="B328" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D328" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E328" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="G328">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E329" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="G329">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="330" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A330" t="s">
+        <v>806</v>
+      </c>
+      <c r="B330" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D330" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E330" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="G330">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="331" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="E331" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="G331">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="332" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A332" t="s">
+        <v>806</v>
+      </c>
+      <c r="B332" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D332" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E332" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="G332">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="E333" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="G333">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A334" t="s">
+        <v>806</v>
+      </c>
+      <c r="B334" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D334" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E334" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="G334">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E335" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="G335">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7" ht="156.6" x14ac:dyDescent="0.4">
+      <c r="A336" t="s">
+        <v>806</v>
+      </c>
+      <c r="B336" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D336" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E336" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="G336">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="E337" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="G337">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A338" t="s">
+        <v>806</v>
+      </c>
+      <c r="B338" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D338" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E338" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="G338">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="E339" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="G339">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A340" t="s">
+        <v>806</v>
+      </c>
+      <c r="B340" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D340" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E340" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="G340">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="E341" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="G341">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A342" t="s">
+        <v>806</v>
+      </c>
+      <c r="B342" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D342" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E342" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="G342">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="E343" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="G343">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A344" t="s">
+        <v>806</v>
+      </c>
+      <c r="B344" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D344" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="E344" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="G344">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="E345" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="G345">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A346" t="s">
+        <v>806</v>
+      </c>
+      <c r="B346" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D346" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E346" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="G346">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="E347" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="G347">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="348" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A348" t="s">
+        <v>806</v>
+      </c>
+      <c r="B348" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D348" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E348" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="G348">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="349" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="E349" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="G349">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="350" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A350" t="s">
+        <v>806</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D350" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E350" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="G350">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="351" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E351" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="G351">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="352" spans="1:7" ht="174" x14ac:dyDescent="0.4">
+      <c r="A352" t="s">
+        <v>806</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D352" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E352" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="G352">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="353" spans="1:7" ht="156.6" x14ac:dyDescent="0.4">
+      <c r="E353" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="G353">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="354" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A354" t="s">
+        <v>806</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D354" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E354" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="G354">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="E355" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="G355">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="356" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A356" t="s">
+        <v>806</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D356" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E356" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="G356">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="E357" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="G357">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A358" t="s">
+        <v>806</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D358" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E358" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="G358">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="E359" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="G359">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="360" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A360" t="s">
+        <v>806</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D360" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E360" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="G360">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E361" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="G361">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="362" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A362" t="s">
+        <v>806</v>
+      </c>
+      <c r="B362" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C362" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D362" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E362" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="G362">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="363" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="E363" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="G363">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="364" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A364" t="s">
+        <v>806</v>
+      </c>
+      <c r="B364" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D364" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E364" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="G364">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="365" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="E365" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="G365">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="366" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A366" t="s">
+        <v>806</v>
+      </c>
+      <c r="B366" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D366" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E366" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="G366">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="367" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="E367" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="G367">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="368" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A368" t="s">
+        <v>806</v>
+      </c>
+      <c r="B368" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C368" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D368" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E368" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="G368">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="369" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="E369" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="G369">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" spans="1:7" ht="139.19999999999999" x14ac:dyDescent="0.4">
+      <c r="A370" t="s">
+        <v>806</v>
+      </c>
+      <c r="B370" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D370" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E370" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="G370">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="371" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="E371" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="G371">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="372" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A372" t="s">
+        <v>806</v>
+      </c>
+      <c r="B372" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D372" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E372" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="G372">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="373" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="E373" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="G373">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="374" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A374" t="s">
+        <v>806</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D374" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E374" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="G374">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="375" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="E375" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="G375">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="376" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A376" t="s">
+        <v>806</v>
+      </c>
+      <c r="B376" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C376" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D376" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E376" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="G376">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="E377" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="G377">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="378" spans="1:7" ht="156.6" x14ac:dyDescent="0.4">
+      <c r="A378" t="s">
+        <v>806</v>
+      </c>
+      <c r="B378" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D378" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E378" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="G378">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="E379" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="G379">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="380" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A380" t="s">
+        <v>806</v>
+      </c>
+      <c r="B380" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D380" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E380" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="G380">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="381" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="E381" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="G381">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="382" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A382" t="s">
+        <v>806</v>
+      </c>
+      <c r="B382" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C382" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D382" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E382" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="G382">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="383" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="E383" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="G383">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="384" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A384" t="s">
+        <v>806</v>
+      </c>
+      <c r="B384" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C384" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D384" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E384" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="G384">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="385" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="E385" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="G385">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="386" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A386" t="s">
+        <v>806</v>
+      </c>
+      <c r="B386" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C386" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D386" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="E386" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="G386">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="387" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="E387" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="G387">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="388" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A388" t="s">
+        <v>806</v>
+      </c>
+      <c r="B388" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C388" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D388" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E388" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="G388">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="389" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="E389" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="G389">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="390" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A390" t="s">
+        <v>806</v>
+      </c>
+      <c r="B390" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C390" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D390" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E390" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="G390">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="391" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="E391" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="G391">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="392" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A392" t="s">
+        <v>806</v>
+      </c>
+      <c r="B392" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C392" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D392" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E392" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="G392">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="393" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="E393" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="G393">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="394" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A394" t="s">
+        <v>806</v>
+      </c>
+      <c r="B394" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D394" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E394" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="G394">
+        <v>0.65</v>
+      </c>
+    </row>
+    <row r="395" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="E395" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="G395">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="396" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A396" t="s">
+        <v>806</v>
+      </c>
+      <c r="B396" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D396" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E396" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="G396">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="397" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="E397" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="G397">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="398" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A398" t="s">
+        <v>806</v>
+      </c>
+      <c r="B398" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C398" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D398" s="1" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="400" spans="1:7" ht="139.19999999999999" x14ac:dyDescent="0.4">
+      <c r="A400" t="s">
+        <v>806</v>
+      </c>
+      <c r="B400" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C400" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D400" s="1" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A402" t="s">
+        <v>806</v>
+      </c>
+      <c r="B402" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C402" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D402" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" ht="87" x14ac:dyDescent="0.4">
+      <c r="A404" t="s">
+        <v>806</v>
+      </c>
+      <c r="B404" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C404" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D404" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A406" t="s">
+        <v>806</v>
+      </c>
+      <c r="B406" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C406" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D406" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" ht="87" x14ac:dyDescent="0.4">
+      <c r="A408" t="s">
+        <v>806</v>
+      </c>
+      <c r="B408" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C408" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D408" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A410" t="s">
+        <v>806</v>
+      </c>
+      <c r="B410" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C410" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D410" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" ht="87" x14ac:dyDescent="0.4">
+      <c r="A412" t="s">
+        <v>806</v>
+      </c>
+      <c r="B412" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C412" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D412" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" ht="156.6" x14ac:dyDescent="0.4">
+      <c r="A414" t="s">
+        <v>806</v>
+      </c>
+      <c r="B414" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C414" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D414" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="416" spans="1:4" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A416" t="s">
+        <v>806</v>
+      </c>
+      <c r="B416" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C416" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D416" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="418" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A418" t="s">
+        <v>806</v>
+      </c>
+      <c r="B418" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C418" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D418" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="420" spans="1:4" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A420" t="s">
+        <v>806</v>
+      </c>
+      <c r="B420" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C420" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D420" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="422" spans="1:4" ht="87" x14ac:dyDescent="0.4">
+      <c r="A422" t="s">
+        <v>806</v>
+      </c>
+      <c r="B422" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C422" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D422" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="424" spans="1:4" ht="87" x14ac:dyDescent="0.4">
+      <c r="A424" t="s">
+        <v>806</v>
+      </c>
+      <c r="B424" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C424" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D424" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="426" spans="1:4" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A426" t="s">
+        <v>806</v>
+      </c>
+      <c r="B426" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C426" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D426" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="428" spans="1:4" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A428" t="s">
+        <v>806</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C428" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D428" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ADD: ML quiz valid dataset (2)
</commit_message>
<xml_diff>
--- a/2025_07_02_OhLoRA_ML_Tutor/ai_quiz/dataset/all_train_and_test_data.xlsx
+++ b/2025_07_02_OhLoRA_ML_Tutor/ai_quiz/dataset/all_train_and_test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB91AE8-C31D-4992-9EFB-04601338525D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012EAF5A-1910-459D-9782-7F2EB57C8553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{07338742-8F51-42F9-A75F-1FCFBE7C4D0C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="879">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1499" uniqueCount="911">
   <si>
     <t>quiz</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -7403,10 +7403,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>valid</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>코사인 유사도는 벡터의 방향을 가지고 판단하는 유사도이다. 벡터 방향이 일치할수록 +1.0, 반대 방향일수록 -1.0에 가까운 값을 갖는다. 코사인 유사도는 S-BERT, 추천 시스템 등에서 사용한다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7692,6 +7688,138 @@
   </si>
   <si>
     <t>드롭아웃은 신경망에서 각 뉴런을 일정 확률로 독립적으로 제거하는 것을 말한다. 오버피팅을 막는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Regularization 은 overfitting 방지를 위해 Loss Function 에 weight 의 절댓값이나 제곱 같은 새로운 항을 추가하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Regularization 은 overfitting 방지를 위해 Loss Function 에 weight 의 절댓값 (L1 regularization) 이나 제곱 (L2 regularization) 의 평균을 새로운 항으로 추가하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Batch Normalization (배치 정규화) 은 딥러닝의 특정 레이어에서, batch 내에 있는 데이터에 대해, 해당 레이어에서의 신경망 내에서의 위치가 동일한 feature 값끼리 평균과 표준편차를 구해서 정규화하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Layer Normalization (레이어 정규화) 은 특정 레이어에서 각 sample 에 해당하는 모든 feature 값에 대해, 동일한 sample 에 해당하는 feature 값끼리 평균과 표준편차를 구해서 정규화하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전이학습은 사전학습된 모델을 가져다가 해당 모델을 적용 가능한 우리의 task 를 학습시키기 위해, 우리의 task 에 대한 데이터셋으로 추가 학습시키는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fine-Tuning 은 전이학습의 핵심으로, 이미 학습된 모델을 우리의 task 에 적용하여 추가 학습시키는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전이학습은 기존 학습된 모델과 새로 학습할 모델 간 데이터셋의 분야가 서로 다를 수 있지만 지식 증류는 경량화 목적이므로 같다. 전이학습은 자원을 절약하며 우리의 task 를 학습시키는 목적이지만 지식 증류는 모델을 경량화시켜 추론 속도를 보다 빠르게 만드는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지식 증류는 모델을 경량화하는 것이고, 전이학습은 기존 모델을 우리의 분야로 전이시켜 추가 학습하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xavier 와 He 는 특정 레이어와 관련된 node 의 개수의 합이 많을수록 해당 레이어를 초기화할 때 파라미터의 평균적인 절댓값 크기가 작아지도록 초기화하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Xavier 와 He 는 특정 레이어와 관련된 node 의 개수의 합이 많을수록 해당 레이어를 초기화할 때 파라미터의 평균적인 절댓값 크기가 작아지도록 초기화하는 것이다. 이때 Xavier 는 입력+출력 노드 개수의 합, He 는 입력 노드 개수만을 고려한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>활성화 함수는 딥러닝의 비선형성을 위해 필요하다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>활성화 함수가 있어야지 입력과 출력 간의 비선형성을 잘 표현할 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multi-Class 분류에서는 Softmax, Multi-Label 분류에서는 각 Class 별 0~1의 확률을 예측하는 Sigmoid 활성화 함수가 적절하다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Multi-Class 분류에서는 Class의 확률이 서로 경쟁하므로 Softmax, Multi-Label 분류에서는 각 Class 별로 독립적으로 예측하여 경쟁성이 없으므로 0~1의 확률을 예측하는 Sigmoid 활성화 함수가 적절하다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oh-LoRA 의 약자이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Low-Rank Adaption 이고 기존 LLM 의 사전학습된 행렬을 2개의 저차원 행렬로 분해해서 해당 저차원 행렬들만 학습시키는 방법이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>top-k, top-p, temperature 는 각각 확률이 가장 큰 k개의 토큰, 누적 확률이 p 이상이 되는 토큰까지 중에서 하나를 선택하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temperature를 1보다 크게 하면 LLM의 출력 토큰이 다양하게 나오고, 1보다 작게 하면 다양하지 않고 특정 토큰만 계속 나오는 듯한 현상이 발생한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DPO = Direct Performance Optimization, ORPO = Odds Ratio Performance Optimization 이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DPO와 ORPO는 각각 Direct Performance Optimization, Odds Ratio Performance Optimization 의 약자이다. 둘 다 선호하는 응답의 확률을 높이고 선호하지 않는 응답의 확률을 줄이는 아이디어이다. DPO는 다른 거대 언어 모델인 참조 모델 (reference model) 을 이용하여, ORPO는 참조 모델 없이 LLM 자체적으로 보유하고 있는 사용자 선호도 데이터를 이용하여 학습하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환각 현상은 LLM이 너처럼 잘못된 답변을 생성하는 것이다. 그래서 사용자에게 오해를 불러일으킨다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>환각 현상은 LLM이 너처럼 잘못된 답변을 생성하는 것이다. 그래서 심각한 경우에는 LLM의 AI 윤리 문제로까지 번질 수 있는 크리티컬한 문제이니 반드시 해결해야 한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retrieval Augmentation 의 약자이다. LLM 을 외부 DB와 연동하여 답변하게 하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Retrieval Augmented Generation 의 약자이다. LLM 을 외부 DB와 연동하여 답변하게 하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PEFT 는 대부분의 파라미터를 얼린 다음 일부분의 파라미터만을 학습해서 OOM을 방지하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Parameter-Efficient Fine-Tuning 으로 그 안에는 너 Oh-LoRA 의 상징인 LoRA, 그리고 QLoRA, Prefix Tuning, Prompt Tuning, 그리고 Adapter Layer 를 추가하는 것이 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quantization 은 양자화로, LLM의 가중치나 활성화 값 같은 값들을 자료형을 바꿔서 메모리에서 차지하는 크기를 줄이는 것이다. 이를 통해 모델 크기 감소, 메모리 양 감소, 추론 시간 단축 등의 효과를 볼 수 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>양자화이며, OOM을 해결한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토큰은 형태소이고 토크나이저는 문장을 형태소 단위로 바꾸는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>토큰은 LLM이나 NLP 모델이 인식하는 일종의 형태소이다. 토크나이저는 문장을 이러한 형태소 단위의 시퀀스로 변환하는 것이다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encoder Self-Attention, Decoder Self-Attention, Encoder-Decoder Self-Attention 이 있다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Encoder Self-Attention, Decoder Self-Attention, Encoder-Decoder Self-Attention 이 있다. Encoder Self-Attention 은 입력되는 문장 (LLM 의 프롬프트) 에서 각 단어의 관계를 (자기 자신 포함) 고려하는 로직이다. Decoder Self Attention은 출력 시퀀스의 각 단어에 대해 입력 시퀀스의 각 단어와의 관계를 고려한다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>valid/test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -8075,10 +8203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF56922-B03A-4496-8414-3644939C6218}">
-  <dimension ref="A1:G428"/>
+  <dimension ref="A1:G429"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A392" workbookViewId="0">
-      <selection activeCell="E398" sqref="E398"/>
+    <sheetView tabSelected="1" topLeftCell="A322" workbookViewId="0">
+      <selection activeCell="B329" sqref="B329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -13121,7 +13249,7 @@
     </row>
     <row r="326" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A326" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B326" s="1" t="s">
         <v>3</v>
@@ -13133,7 +13261,7 @@
         <v>4</v>
       </c>
       <c r="E326" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="G326">
         <v>0.9</v>
@@ -13141,10 +13269,10 @@
     </row>
     <row r="327" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A327" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="E327" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="G327">
         <v>0.15</v>
@@ -13152,7 +13280,7 @@
     </row>
     <row r="328" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
       <c r="A328" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B328" s="1" t="s">
         <v>5</v>
@@ -13164,15 +13292,18 @@
         <v>6</v>
       </c>
       <c r="E328" s="1" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G328">
         <v>0.8</v>
       </c>
     </row>
     <row r="329" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A329" t="s">
+        <v>910</v>
+      </c>
       <c r="E329" s="1" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G329">
         <v>0.2</v>
@@ -13180,7 +13311,7 @@
     </row>
     <row r="330" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A330" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B330" s="1" t="s">
         <v>7</v>
@@ -13192,15 +13323,18 @@
         <v>8</v>
       </c>
       <c r="E330" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="G330">
         <v>0.5</v>
       </c>
     </row>
     <row r="331" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A331" t="s">
+        <v>910</v>
+      </c>
       <c r="E331" s="1" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="G331">
         <v>0.15</v>
@@ -13208,7 +13342,7 @@
     </row>
     <row r="332" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
       <c r="A332" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B332" s="1" t="s">
         <v>9</v>
@@ -13220,15 +13354,18 @@
         <v>10</v>
       </c>
       <c r="E332" s="1" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="G332">
         <v>0.4</v>
       </c>
     </row>
     <row r="333" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A333" t="s">
+        <v>910</v>
+      </c>
       <c r="E333" s="1" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="G333">
         <v>0.6</v>
@@ -13236,7 +13373,7 @@
     </row>
     <row r="334" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A334" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B334" s="1" t="s">
         <v>11</v>
@@ -13248,15 +13385,18 @@
         <v>12</v>
       </c>
       <c r="E334" s="1" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="G334">
         <v>1</v>
       </c>
     </row>
     <row r="335" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A335" t="s">
+        <v>910</v>
+      </c>
       <c r="E335" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="G335">
         <v>0.45</v>
@@ -13264,7 +13404,7 @@
     </row>
     <row r="336" spans="1:7" ht="156.6" x14ac:dyDescent="0.4">
       <c r="A336" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B336" s="1" t="s">
         <v>13</v>
@@ -13276,15 +13416,18 @@
         <v>14</v>
       </c>
       <c r="E336" s="1" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="G336">
         <v>1</v>
       </c>
     </row>
     <row r="337" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A337" t="s">
+        <v>910</v>
+      </c>
       <c r="E337" s="1" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G337">
         <v>0.2</v>
@@ -13292,7 +13435,7 @@
     </row>
     <row r="338" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A338" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B338" s="1" t="s">
         <v>15</v>
@@ -13304,15 +13447,18 @@
         <v>16</v>
       </c>
       <c r="E338" s="1" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G338">
         <v>1</v>
       </c>
     </row>
     <row r="339" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A339" t="s">
+        <v>910</v>
+      </c>
       <c r="E339" s="1" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="G339">
         <v>0.4</v>
@@ -13320,7 +13466,7 @@
     </row>
     <row r="340" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A340" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B340" s="1" t="s">
         <v>17</v>
@@ -13332,15 +13478,18 @@
         <v>18</v>
       </c>
       <c r="E340" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="G340">
         <v>0.5</v>
       </c>
     </row>
     <row r="341" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A341" t="s">
+        <v>910</v>
+      </c>
       <c r="E341" s="1" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="G341">
         <v>0.35</v>
@@ -13348,7 +13497,7 @@
     </row>
     <row r="342" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A342" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B342" s="1" t="s">
         <v>19</v>
@@ -13360,15 +13509,18 @@
         <v>20</v>
       </c>
       <c r="E342" s="1" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="G342">
         <v>1</v>
       </c>
     </row>
     <row r="343" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A343" t="s">
+        <v>910</v>
+      </c>
       <c r="E343" s="1" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="G343">
         <v>0.3</v>
@@ -13376,7 +13528,7 @@
     </row>
     <row r="344" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
       <c r="A344" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B344" s="1" t="s">
         <v>21</v>
@@ -13388,15 +13540,18 @@
         <v>432</v>
       </c>
       <c r="E344" s="1" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="G344">
         <v>0.35</v>
       </c>
     </row>
     <row r="345" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A345" t="s">
+        <v>910</v>
+      </c>
       <c r="E345" s="1" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="G345">
         <v>0.75</v>
@@ -13404,7 +13559,7 @@
     </row>
     <row r="346" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A346" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B346" s="1" t="s">
         <v>22</v>
@@ -13416,15 +13571,18 @@
         <v>23</v>
       </c>
       <c r="E346" s="1" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="G346">
         <v>1</v>
       </c>
     </row>
     <row r="347" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A347" t="s">
+        <v>910</v>
+      </c>
       <c r="E347" s="1" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="G347">
         <v>0.35</v>
@@ -13432,7 +13590,7 @@
     </row>
     <row r="348" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
       <c r="A348" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B348" s="1" t="s">
         <v>24</v>
@@ -13444,15 +13602,18 @@
         <v>25</v>
       </c>
       <c r="E348" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="G348">
         <v>0.75</v>
       </c>
     </row>
     <row r="349" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A349" t="s">
+        <v>910</v>
+      </c>
       <c r="E349" s="1" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G349">
         <v>0.3</v>
@@ -13460,7 +13621,7 @@
     </row>
     <row r="350" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A350" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B350" s="1" t="s">
         <v>26</v>
@@ -13472,15 +13633,18 @@
         <v>37</v>
       </c>
       <c r="E350" s="1" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="G350">
         <v>0.6</v>
       </c>
     </row>
     <row r="351" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A351" t="s">
+        <v>910</v>
+      </c>
       <c r="E351" s="1" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="G351">
         <v>0.3</v>
@@ -13488,7 +13652,7 @@
     </row>
     <row r="352" spans="1:7" ht="174" x14ac:dyDescent="0.4">
       <c r="A352" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B352" s="1" t="s">
         <v>38</v>
@@ -13500,15 +13664,18 @@
         <v>39</v>
       </c>
       <c r="E352" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="G352">
         <v>0.75</v>
       </c>
     </row>
     <row r="353" spans="1:7" ht="156.6" x14ac:dyDescent="0.4">
+      <c r="A353" t="s">
+        <v>910</v>
+      </c>
       <c r="E353" s="1" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="G353">
         <v>0.1</v>
@@ -13516,7 +13683,7 @@
     </row>
     <row r="354" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A354" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B354" s="1" t="s">
         <v>42</v>
@@ -13528,15 +13695,18 @@
         <v>43</v>
       </c>
       <c r="E354" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="G354">
         <v>1</v>
       </c>
     </row>
     <row r="355" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A355" t="s">
+        <v>910</v>
+      </c>
       <c r="E355" s="1" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="G355">
         <v>0.3</v>
@@ -13544,7 +13714,7 @@
     </row>
     <row r="356" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A356" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B356" s="1" t="s">
         <v>45</v>
@@ -13556,15 +13726,18 @@
         <v>46</v>
       </c>
       <c r="E356" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="G356">
         <v>0.2</v>
       </c>
     </row>
     <row r="357" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A357" t="s">
+        <v>910</v>
+      </c>
       <c r="E357" s="1" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="G357">
         <v>0.65</v>
@@ -13572,7 +13745,7 @@
     </row>
     <row r="358" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A358" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B358" s="1" t="s">
         <v>48</v>
@@ -13584,15 +13757,18 @@
         <v>50</v>
       </c>
       <c r="E358" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="G358">
         <v>0.1</v>
       </c>
     </row>
     <row r="359" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A359" t="s">
+        <v>910</v>
+      </c>
       <c r="E359" s="1" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="G359">
         <v>1</v>
@@ -13600,7 +13776,7 @@
     </row>
     <row r="360" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A360" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>52</v>
@@ -13612,15 +13788,18 @@
         <v>53</v>
       </c>
       <c r="E360" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="G360">
         <v>0</v>
       </c>
     </row>
     <row r="361" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A361" t="s">
+        <v>910</v>
+      </c>
       <c r="E361" s="1" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="G361">
         <v>0.1</v>
@@ -13628,7 +13807,7 @@
     </row>
     <row r="362" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A362" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B362" s="1" t="s">
         <v>55</v>
@@ -13640,15 +13819,18 @@
         <v>57</v>
       </c>
       <c r="E362" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="G362">
         <v>0.4</v>
       </c>
     </row>
     <row r="363" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A363" t="s">
+        <v>910</v>
+      </c>
       <c r="E363" s="1" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G363">
         <v>0.65</v>
@@ -13656,7 +13838,7 @@
     </row>
     <row r="364" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A364" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B364" s="1" t="s">
         <v>58</v>
@@ -13668,15 +13850,18 @@
         <v>59</v>
       </c>
       <c r="E364" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="G364">
         <v>0.6</v>
       </c>
     </row>
     <row r="365" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A365" t="s">
+        <v>910</v>
+      </c>
       <c r="E365" s="1" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="G365">
         <v>0.6</v>
@@ -13684,7 +13869,7 @@
     </row>
     <row r="366" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A366" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B366" s="1" t="s">
         <v>61</v>
@@ -13696,15 +13881,18 @@
         <v>62</v>
       </c>
       <c r="E366" s="1" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G366">
         <v>0</v>
       </c>
     </row>
     <row r="367" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A367" t="s">
+        <v>910</v>
+      </c>
       <c r="E367" s="1" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="G367">
         <v>1</v>
@@ -13712,7 +13900,7 @@
     </row>
     <row r="368" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A368" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B368" s="1" t="s">
         <v>64</v>
@@ -13724,15 +13912,18 @@
         <v>65</v>
       </c>
       <c r="E368" s="1" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="G368">
         <v>0.5</v>
       </c>
     </row>
     <row r="369" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A369" t="s">
+        <v>910</v>
+      </c>
       <c r="E369" s="1" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="G369">
         <v>1</v>
@@ -13740,7 +13931,7 @@
     </row>
     <row r="370" spans="1:7" ht="139.19999999999999" x14ac:dyDescent="0.4">
       <c r="A370" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B370" s="1" t="s">
         <v>68</v>
@@ -13752,15 +13943,18 @@
         <v>67</v>
       </c>
       <c r="E370" s="1" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="G370">
         <v>0</v>
       </c>
     </row>
     <row r="371" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A371" t="s">
+        <v>910</v>
+      </c>
       <c r="E371" s="1" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="G371">
         <v>0.7</v>
@@ -13768,7 +13962,7 @@
     </row>
     <row r="372" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
       <c r="A372" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B372" s="1" t="s">
         <v>70</v>
@@ -13780,15 +13974,18 @@
         <v>72</v>
       </c>
       <c r="E372" s="1" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G372">
         <v>0.1</v>
       </c>
     </row>
     <row r="373" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A373" t="s">
+        <v>910</v>
+      </c>
       <c r="E373" s="1" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G373">
         <v>1</v>
@@ -13796,7 +13993,7 @@
     </row>
     <row r="374" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A374" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B374" s="1" t="s">
         <v>73</v>
@@ -13808,15 +14005,18 @@
         <v>74</v>
       </c>
       <c r="E374" s="1" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="G374">
         <v>0.4</v>
       </c>
     </row>
     <row r="375" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A375" t="s">
+        <v>910</v>
+      </c>
       <c r="E375" s="1" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="G375">
         <v>0</v>
@@ -13824,7 +14024,7 @@
     </row>
     <row r="376" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A376" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B376" s="1" t="s">
         <v>75</v>
@@ -13836,15 +14036,18 @@
         <v>76</v>
       </c>
       <c r="E376" s="1" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="G376">
         <v>1</v>
       </c>
     </row>
     <row r="377" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A377" t="s">
+        <v>910</v>
+      </c>
       <c r="E377" s="1" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="G377">
         <v>0.85</v>
@@ -13852,7 +14055,7 @@
     </row>
     <row r="378" spans="1:7" ht="156.6" x14ac:dyDescent="0.4">
       <c r="A378" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B378" s="1" t="s">
         <v>78</v>
@@ -13864,15 +14067,18 @@
         <v>79</v>
       </c>
       <c r="E378" s="1" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="G378">
         <v>0</v>
       </c>
     </row>
     <row r="379" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A379" t="s">
+        <v>910</v>
+      </c>
       <c r="E379" s="1" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="G379">
         <v>0.3</v>
@@ -13880,7 +14086,7 @@
     </row>
     <row r="380" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A380" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B380" s="1" t="s">
         <v>83</v>
@@ -13892,15 +14098,18 @@
         <v>81</v>
       </c>
       <c r="E380" s="1" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G380">
         <v>0.25</v>
       </c>
     </row>
     <row r="381" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A381" t="s">
+        <v>910</v>
+      </c>
       <c r="E381" s="1" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G381">
         <v>0.65</v>
@@ -13908,7 +14117,7 @@
     </row>
     <row r="382" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A382" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B382" s="1" t="s">
         <v>85</v>
@@ -13920,15 +14129,18 @@
         <v>84</v>
       </c>
       <c r="E382" s="1" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="G382">
         <v>0</v>
       </c>
     </row>
     <row r="383" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A383" t="s">
+        <v>910</v>
+      </c>
       <c r="E383" s="1" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G383">
         <v>0.5</v>
@@ -13936,7 +14148,7 @@
     </row>
     <row r="384" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A384" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B384" s="1" t="s">
         <v>87</v>
@@ -13948,15 +14160,18 @@
         <v>88</v>
       </c>
       <c r="E384" s="1" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G384">
         <v>0.15</v>
       </c>
     </row>
     <row r="385" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A385" t="s">
+        <v>910</v>
+      </c>
       <c r="E385" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G385">
         <v>1</v>
@@ -13964,7 +14179,7 @@
     </row>
     <row r="386" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A386" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B386" s="1" t="s">
         <v>90</v>
@@ -13976,15 +14191,18 @@
         <v>91</v>
       </c>
       <c r="E386" s="1" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="G386">
         <v>0.4</v>
       </c>
     </row>
     <row r="387" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A387" t="s">
+        <v>910</v>
+      </c>
       <c r="E387" s="1" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="G387">
         <v>0.5</v>
@@ -13992,7 +14210,7 @@
     </row>
     <row r="388" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A388" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B388" s="1" t="s">
         <v>93</v>
@@ -14004,15 +14222,18 @@
         <v>94</v>
       </c>
       <c r="E388" s="1" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G388">
         <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="389" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A389" t="s">
+        <v>910</v>
+      </c>
       <c r="E389" s="1" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="G389">
         <v>0.75</v>
@@ -14020,7 +14241,7 @@
     </row>
     <row r="390" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A390" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B390" s="1" t="s">
         <v>96</v>
@@ -14032,15 +14253,18 @@
         <v>97</v>
       </c>
       <c r="E390" s="1" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="G390">
         <v>0</v>
       </c>
     </row>
     <row r="391" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A391" t="s">
+        <v>910</v>
+      </c>
       <c r="E391" s="1" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="G391">
         <v>0.25</v>
@@ -14048,7 +14272,7 @@
     </row>
     <row r="392" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A392" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B392" s="1" t="s">
         <v>100</v>
@@ -14060,15 +14284,18 @@
         <v>99</v>
       </c>
       <c r="E392" s="1" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="G392">
         <v>0.3</v>
       </c>
     </row>
     <row r="393" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A393" t="s">
+        <v>910</v>
+      </c>
       <c r="E393" s="1" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="G393">
         <v>0.6</v>
@@ -14076,7 +14303,7 @@
     </row>
     <row r="394" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
       <c r="A394" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B394" s="1" t="s">
         <v>102</v>
@@ -14088,15 +14315,18 @@
         <v>103</v>
       </c>
       <c r="E394" s="1" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="G394">
         <v>0.65</v>
       </c>
     </row>
     <row r="395" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A395" t="s">
+        <v>910</v>
+      </c>
       <c r="E395" s="1" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="G395">
         <v>0.6</v>
@@ -14104,7 +14334,7 @@
     </row>
     <row r="396" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A396" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B396" s="1" t="s">
         <v>105</v>
@@ -14116,15 +14346,18 @@
         <v>104</v>
       </c>
       <c r="E396" s="1" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="G396">
         <v>0.5</v>
       </c>
     </row>
     <row r="397" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A397" t="s">
+        <v>910</v>
+      </c>
       <c r="E397" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="G397">
         <v>0.8</v>
@@ -14132,7 +14365,7 @@
     </row>
     <row r="398" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A398" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B398" s="1" t="s">
         <v>107</v>
@@ -14143,10 +14376,27 @@
       <c r="D398" s="1" t="s">
         <v>663</v>
       </c>
+      <c r="E398" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="G398">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="399" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A399" t="s">
+        <v>910</v>
+      </c>
+      <c r="E399" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="G399">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="400" spans="1:7" ht="139.19999999999999" x14ac:dyDescent="0.4">
       <c r="A400" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B400" s="1" t="s">
         <v>108</v>
@@ -14157,10 +14407,27 @@
       <c r="D400" s="1" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="402" spans="1:4" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="E400" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="G400">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="401" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A401" t="s">
+        <v>910</v>
+      </c>
+      <c r="E401" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="G401">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="402" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A402" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B402" s="1" t="s">
         <v>109</v>
@@ -14171,10 +14438,27 @@
       <c r="D402" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="404" spans="1:4" ht="87" x14ac:dyDescent="0.4">
+      <c r="E402" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="G402">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A403" t="s">
+        <v>910</v>
+      </c>
+      <c r="E403" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="G403">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="404" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A404" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B404" s="1" t="s">
         <v>112</v>
@@ -14185,10 +14469,27 @@
       <c r="D404" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="406" spans="1:4" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="E404" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="G404">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="405" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A405" t="s">
+        <v>910</v>
+      </c>
+      <c r="E405" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="G405">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="406" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A406" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B406" s="1" t="s">
         <v>116</v>
@@ -14199,10 +14500,27 @@
       <c r="D406" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="408" spans="1:4" ht="87" x14ac:dyDescent="0.4">
+      <c r="E406" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="G406">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="407" spans="1:7" ht="87" x14ac:dyDescent="0.4">
+      <c r="A407" t="s">
+        <v>910</v>
+      </c>
+      <c r="E407" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="G407">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A408" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B408" s="1" t="s">
         <v>122</v>
@@ -14213,10 +14531,27 @@
       <c r="D408" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="410" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="E408" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="G408">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="409" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A409" t="s">
+        <v>910</v>
+      </c>
+      <c r="E409" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="G409">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="410" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A410" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B410" s="1" t="s">
         <v>124</v>
@@ -14227,10 +14562,27 @@
       <c r="D410" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="412" spans="1:4" ht="87" x14ac:dyDescent="0.4">
+      <c r="E410" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="G410">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="411" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A411" t="s">
+        <v>910</v>
+      </c>
+      <c r="E411" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="G411">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="412" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A412" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B412" s="1" t="s">
         <v>127</v>
@@ -14241,10 +14593,27 @@
       <c r="D412" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="414" spans="1:4" ht="156.6" x14ac:dyDescent="0.4">
+      <c r="E412" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="G412">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="413" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A413" t="s">
+        <v>910</v>
+      </c>
+      <c r="E413" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="G413">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="414" spans="1:7" ht="156.6" x14ac:dyDescent="0.4">
       <c r="A414" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B414" s="1" t="s">
         <v>129</v>
@@ -14255,10 +14624,27 @@
       <c r="D414" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="416" spans="1:4" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="E414" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="G414">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="415" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A415" t="s">
+        <v>910</v>
+      </c>
+      <c r="E415" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="G415">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="416" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A416" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B416" s="1" t="s">
         <v>131</v>
@@ -14269,10 +14655,27 @@
       <c r="D416" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="418" spans="1:4" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="E416" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="G416">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="417" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="A417" t="s">
+        <v>910</v>
+      </c>
+      <c r="E417" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="G417">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="418" spans="1:7" ht="69.599999999999994" x14ac:dyDescent="0.4">
       <c r="A418" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B418" s="1" t="s">
         <v>136</v>
@@ -14283,10 +14686,27 @@
       <c r="D418" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="420" spans="1:4" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="E418" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="G418">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="419" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A419" t="s">
+        <v>910</v>
+      </c>
+      <c r="E419" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="G419">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="420" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
       <c r="A420" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B420" s="1" t="s">
         <v>140</v>
@@ -14297,10 +14717,27 @@
       <c r="D420" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="422" spans="1:4" ht="87" x14ac:dyDescent="0.4">
+      <c r="E420" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="G420">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="421" spans="1:7" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A421" t="s">
+        <v>910</v>
+      </c>
+      <c r="E421" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="G421">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="422" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A422" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B422" s="1" t="s">
         <v>143</v>
@@ -14311,10 +14748,27 @@
       <c r="D422" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="424" spans="1:4" ht="87" x14ac:dyDescent="0.4">
+      <c r="E422" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="G422">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="423" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A423" t="s">
+        <v>910</v>
+      </c>
+      <c r="E423" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="G423">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" spans="1:7" ht="87" x14ac:dyDescent="0.4">
       <c r="A424" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B424" s="1" t="s">
         <v>146</v>
@@ -14325,10 +14779,27 @@
       <c r="D424" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="426" spans="1:4" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="E424" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="G424">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="425" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A425" t="s">
+        <v>910</v>
+      </c>
+      <c r="E425" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="G425">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="426" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A426" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B426" s="1" t="s">
         <v>149</v>
@@ -14339,10 +14810,27 @@
       <c r="D426" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="428" spans="1:4" ht="121.8" x14ac:dyDescent="0.4">
+      <c r="E426" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="G426">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="427" spans="1:7" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A427" t="s">
+        <v>910</v>
+      </c>
+      <c r="E427" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="G427">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="428" spans="1:7" ht="121.8" x14ac:dyDescent="0.4">
       <c r="A428" t="s">
-        <v>806</v>
+        <v>910</v>
       </c>
       <c r="B428" s="1" t="s">
         <v>152</v>
@@ -14352,6 +14840,23 @@
       </c>
       <c r="D428" s="1" t="s">
         <v>153</v>
+      </c>
+      <c r="E428" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="G428">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="429" spans="1:7" ht="104.4" x14ac:dyDescent="0.4">
+      <c r="A429" t="s">
+        <v>910</v>
+      </c>
+      <c r="E429" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="G429">
+        <v>0.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>